<commit_message>
Updated Lists summary spreadsheet and corrected some whitespace in csv files
</commit_message>
<xml_diff>
--- a/analysis/Current-Historical-List-Ids.xlsx
+++ b/analysis/Current-Historical-List-Ids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oco115\PycharmProjects\authoritative-lists\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B353F336-3233-463F-89A0-CB69660A58EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE51C9E-C326-4860-943C-584CDC3EF463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="1755" windowWidth="21210" windowHeight="15195" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="1455" windowWidth="21420" windowHeight="15195" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="191">
   <si>
     <t>Sensitive</t>
   </si>
@@ -595,6 +595,12 @@
   </si>
   <si>
     <t>No new list - region doesn't match</t>
+  </si>
+  <si>
+    <t>dr491</t>
+  </si>
+  <si>
+    <t>TAS</t>
   </si>
 </sst>
 </file>
@@ -1264,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F43AB59-C670-488C-8E62-1F8BBF480EBA}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,74 +1308,74 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F4" t="s">
-        <v>185</v>
+      <c r="C3" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>147</v>
+        <v>152</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>188</v>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>7</v>
+        <v>147</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>145</v>
+        <v>87</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>183</v>
@@ -1389,122 +1395,125 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D9" s="9" t="s">
+    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>183</v>
+      <c r="F9" s="10" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>88</v>
-      </c>
       <c r="F10" s="9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B14" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>136</v>
-      </c>
-      <c r="F17" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F18" t="s">
         <v>185</v>
@@ -1512,41 +1521,41 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="F19" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>141</v>
-      </c>
-      <c r="F20" t="s">
-        <v>185</v>
+    <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F21" t="s">
         <v>185</v>
@@ -1554,61 +1563,89 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F22" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9" t="s">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D26" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F26" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+    <row r="27" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D27" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E27" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F27" s="9" t="s">
         <v>183</v>
       </c>
     </row>
@@ -1622,7 +1659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009932E9-3BF2-4CEF-AF54-2DFB95D312F2}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated DR for EPBCA Conservation in Prod
</commit_message>
<xml_diff>
--- a/analysis/Current-Historical-List-Ids.xlsx
+++ b/analysis/Current-Historical-List-Ids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oco115\PycharmProjects\authoritative-lists\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{69FDABAA-64E8-49DE-B76E-D212E95B30BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA7689A-AC0F-4EF5-AD36-E5D656FE03A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17655" yWindow="3735" windowWidth="28065" windowHeight="15420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="21195" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="314">
   <si>
     <t>Sensitive</t>
   </si>
@@ -965,6 +965,12 @@
   </si>
   <si>
     <t>Authoritative</t>
+  </si>
+  <si>
+    <t>dr18718</t>
+  </si>
+  <si>
+    <t>dr18735</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1075,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1077,12 +1083,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1366,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1383,7 @@
     <col min="3" max="3" width="54.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1487,14 +1494,19 @@
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="13" t="s">
         <v>37</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1534,7 +1546,7 @@
         <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1674,58 +1686,58 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>145</v>
       </c>
       <c r="F2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1743,62 +1755,62 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1816,60 +1828,60 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1906,17 +1918,17 @@
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="8" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1990,34 +2002,34 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+    <row r="25" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="10" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="8" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3031,8 +3043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E1CD31-ADFA-4968-B027-EE786ACAB43C}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update for NSW conservation
</commit_message>
<xml_diff>
--- a/analysis/Current-Historical-List-Ids.xlsx
+++ b/analysis/Current-Historical-List-Ids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oco115\PycharmProjects\authoritative-lists\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA7689A-AC0F-4EF5-AD36-E5D656FE03A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7776A5-4814-4C04-AE9B-53E5794F946A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="21195" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="10185" windowWidth="21195" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="318">
   <si>
     <t>Sensitive</t>
   </si>
@@ -971,6 +971,18 @@
   </si>
   <si>
     <t>dr18735</t>
+  </si>
+  <si>
+    <t>https://lists-test.ala.org.au/speciesListItem/list/dr18437</t>
+  </si>
+  <si>
+    <t>dr18437</t>
+  </si>
+  <si>
+    <t>dr18736</t>
+  </si>
+  <si>
+    <t>https://lists-test.ala.org.au/speciesListItem/list/dr650</t>
   </si>
 </sst>
 </file>
@@ -1371,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,6 +1652,26 @@
         <v>64</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" t="s">
+        <v>317</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F15" t="s">
+        <v>315</v>
+      </c>
+      <c r="G15" t="s">
+        <v>316</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -1647,9 +1679,10 @@
     <hyperlink ref="E2" r:id="rId2" xr:uid="{986401DC-0BF7-4C73-986B-8606D257EF06}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{952BDF74-1025-44CA-B437-CA7A782DEF2C}"/>
     <hyperlink ref="D12" r:id="rId4" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BA5A33AF-C0B9-4DFE-9F12-7BFDF7D8A911}"/>
+    <hyperlink ref="E15" r:id="rId5" xr:uid="{ECFB10CF-9B59-4B58-9F8C-86B26ED2D1A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
compare new conservation lists for the lists-test env
</commit_message>
<xml_diff>
--- a/analysis/Current-Historical-List-Ids.xlsx
+++ b/analysis/Current-Historical-List-Ids.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oco115\PycharmProjects\authoritative-lists\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/new330/IdeaProjects/authoritative-lists/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7776A5-4814-4C04-AE9B-53E5794F946A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479D02A1-A103-A34D-B5EC-C0D112356B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="10185" windowWidth="21195" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59580" yWindow="2520" windowWidth="24900" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="333">
   <si>
     <t>Sensitive</t>
   </si>
@@ -553,9 +553,6 @@
     <t>Test - Current New DR ID</t>
   </si>
   <si>
-    <t>Test - Current - New List</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sensitive </t>
   </si>
   <si>
@@ -983,6 +980,54 @@
   </si>
   <si>
     <t>https://lists-test.ala.org.au/speciesListItem/list/dr650</t>
+  </si>
+  <si>
+    <t>LISTS-TEST ENVIRONMENT</t>
+  </si>
+  <si>
+    <t>LISTS PROD ENVIRONMENT</t>
+  </si>
+  <si>
+    <t>TEMP new list</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr2201</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr649</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr652</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr651</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr656</t>
+  </si>
+  <si>
+    <t>https://lists..ala.org.au/speciesListItem/list/dr653</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr654</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr655</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr650</t>
+  </si>
+  <si>
+    <t>dr18759</t>
+  </si>
+  <si>
+    <t>https://lists-test.ala.org.au/speciesListItem/list/dr18396</t>
+  </si>
+  <si>
+    <t>dr18396</t>
+  </si>
+  <si>
+    <t>https://lists-test.ala.org.au/speciesListItem/list/dr2201</t>
   </si>
 </sst>
 </file>
@@ -1383,306 +1428,531 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="54.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" t="s">
+        <v>316</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F16" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F17" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C24" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D24" t="s">
         <v>35</v>
       </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C25" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B27" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="C27" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12" t="s">
+      <c r="F27" s="12" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C30" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C31" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F31" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="C32" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>4</v>
       </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C33" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="F33" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>176</v>
-      </c>
-      <c r="C15" t="s">
-        <v>317</v>
-      </c>
-      <c r="D15" s="4" t="s">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="F34" t="s">
         <v>315</v>
       </c>
-      <c r="G15" t="s">
-        <v>316</v>
-      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>320</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F35" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" xr:uid="{6EE0F20C-BD06-4978-B8CD-E66E5C646CF8}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{986401DC-0BF7-4C73-986B-8606D257EF06}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{952BDF74-1025-44CA-B437-CA7A782DEF2C}"/>
-    <hyperlink ref="D12" r:id="rId4" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BA5A33AF-C0B9-4DFE-9F12-7BFDF7D8A911}"/>
-    <hyperlink ref="E15" r:id="rId5" xr:uid="{ECFB10CF-9B59-4B58-9F8C-86B26ED2D1A6}"/>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{6EE0F20C-BD06-4978-B8CD-E66E5C646CF8}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{986401DC-0BF7-4C73-986B-8606D257EF06}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{952BDF74-1025-44CA-B437-CA7A782DEF2C}"/>
+    <hyperlink ref="D13" r:id="rId4" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BA5A33AF-C0B9-4DFE-9F12-7BFDF7D8A911}"/>
+    <hyperlink ref="E16" r:id="rId5" xr:uid="{ECFB10CF-9B59-4B58-9F8C-86B26ED2D1A6}"/>
+    <hyperlink ref="C32" r:id="rId6" xr:uid="{D698F75E-C3A9-2E43-9EF9-D03CAFBC8EA9}"/>
+    <hyperlink ref="C22" r:id="rId7" xr:uid="{4780244B-70BF-9C48-970A-9B52EE257B77}"/>
+    <hyperlink ref="D32" r:id="rId8" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BCC2EF75-48CD-4548-9585-233F9187C820}"/>
+    <hyperlink ref="A21" r:id="rId9" xr:uid="{4A0B836D-E3B0-794C-A4F5-21AA69E861E2}"/>
+    <hyperlink ref="A2" r:id="rId10" xr:uid="{6FC89B14-CCA6-C244-9CDE-F11F9F1FF7E7}"/>
+    <hyperlink ref="A8" r:id="rId11" xr:uid="{6366CB73-381F-0249-A1E4-038947A0C509}"/>
+    <hyperlink ref="A27" r:id="rId12" xr:uid="{B8D63856-57FE-8C42-8EAD-AECB4BC1FF98}"/>
+    <hyperlink ref="C27" r:id="rId13" xr:uid="{96429AFB-B264-344B-B15E-8F464D602044}"/>
+    <hyperlink ref="C28" r:id="rId14" xr:uid="{31C2BC7F-43DC-0447-95EB-1702F49CA889}"/>
+    <hyperlink ref="C29" r:id="rId15" xr:uid="{5EF5C7C0-C9E6-624F-BF44-A5738449F8BA}"/>
+    <hyperlink ref="C30" r:id="rId16" xr:uid="{9AA0D4E8-104C-FA40-B731-F1AFD127B25C}"/>
+    <hyperlink ref="C31" r:id="rId17" xr:uid="{0AA1FC7B-6EFA-B54C-A968-3E6832124A77}"/>
+    <hyperlink ref="C33" r:id="rId18" xr:uid="{88BF66EA-B4A9-5B40-A7A3-599D95618642}"/>
+    <hyperlink ref="C34" r:id="rId19" xr:uid="{7A14450F-9C85-3C46-891C-D60F0551E9B5}"/>
+    <hyperlink ref="C17" r:id="rId20" xr:uid="{5A2DA5AE-E509-094D-981A-96E4E13B0899}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -1694,25 +1964,25 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
     <col min="6" max="6" width="44" customWidth="1"/>
-    <col min="7" max="7" width="38.7109375" customWidth="1"/>
+    <col min="7" max="7" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
@@ -1723,24 +1993,24 @@
         <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>140</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>147</v>
       </c>
@@ -1751,16 +2021,16 @@
         <v>148</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>149</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>151</v>
       </c>
@@ -1771,10 +2041,10 @@
         <v>144</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
@@ -1785,10 +2055,10 @@
         <v>138</v>
       </c>
       <c r="F6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>146</v>
       </c>
@@ -1796,10 +2066,10 @@
         <v>86</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>152</v>
       </c>
@@ -1810,44 +2080,44 @@
         <v>141</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>139</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>139</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>36</v>
       </c>
@@ -1858,10 +2128,10 @@
         <v>143</v>
       </c>
       <c r="F11" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>153</v>
       </c>
@@ -1878,10 +2148,10 @@
         <v>96</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>155</v>
       </c>
@@ -1898,10 +2168,10 @@
         <v>87</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>150</v>
       </c>
@@ -1915,15 +2185,15 @@
         <v>96</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
@@ -1934,10 +2204,10 @@
         <v>135</v>
       </c>
       <c r="F17" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
@@ -1948,24 +2218,24 @@
         <v>86</v>
       </c>
       <c r="F18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>136</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>137</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>40</v>
       </c>
@@ -1976,10 +2246,10 @@
         <v>144</v>
       </c>
       <c r="F20" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
@@ -1990,10 +2260,10 @@
         <v>138</v>
       </c>
       <c r="F21" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
@@ -2004,10 +2274,10 @@
         <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
@@ -2018,10 +2288,10 @@
         <v>140</v>
       </c>
       <c r="F23" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>44</v>
       </c>
@@ -2032,10 +2302,10 @@
         <v>139</v>
       </c>
       <c r="F24" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>142</v>
       </c>
@@ -2046,10 +2316,10 @@
         <v>143</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>156</v>
       </c>
@@ -2060,10 +2330,10 @@
         <v>86</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2076,21 +2346,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009932E9-3BF2-4CEF-AF54-2DFB95D312F2}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" customWidth="1"/>
-    <col min="8" max="8" width="44.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="31.1640625" customWidth="1"/>
+    <col min="8" max="8" width="44.5" customWidth="1"/>
+    <col min="9" max="9" width="27.5" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -2131,7 +2401,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -2160,7 +2430,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -2195,7 +2465,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -2227,7 +2497,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -2259,7 +2529,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -2291,7 +2561,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -2323,7 +2593,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -2349,7 +2619,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -2372,7 +2642,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -2395,7 +2665,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -2418,7 +2688,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -2441,7 +2711,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>136</v>
       </c>
@@ -2464,7 +2734,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
@@ -2487,7 +2757,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -2510,7 +2780,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
@@ -2533,7 +2803,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>41</v>
       </c>
@@ -2556,7 +2826,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>142</v>
       </c>
@@ -2579,7 +2849,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
@@ -2602,7 +2872,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -2625,7 +2895,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>146</v>
       </c>
@@ -2648,7 +2918,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>147</v>
       </c>
@@ -2680,7 +2950,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>150</v>
       </c>
@@ -2709,7 +2979,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>151</v>
       </c>
@@ -2732,7 +3002,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
@@ -2755,7 +3025,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>152</v>
       </c>
@@ -2778,7 +3048,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -2801,7 +3071,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>153</v>
       </c>
@@ -2833,7 +3103,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>155</v>
       </c>
@@ -2865,7 +3135,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>156</v>
       </c>
@@ -2891,7 +3161,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>158</v>
       </c>
@@ -2917,7 +3187,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>160</v>
       </c>
@@ -2943,7 +3213,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>161</v>
       </c>
@@ -2969,7 +3239,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>162</v>
       </c>
@@ -2995,7 +3265,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>166</v>
       </c>
@@ -3018,7 +3288,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>167</v>
       </c>
@@ -3041,7 +3311,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>168</v>
       </c>
@@ -3080,755 +3350,755 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1"/>
-    <col min="5" max="5" width="48.85546875" customWidth="1"/>
+    <col min="1" max="1" width="53.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="70.5" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="5" max="5" width="48.83203125" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" customWidth="1"/>
-    <col min="12" max="12" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.5" customWidth="1"/>
+    <col min="10" max="10" width="24.83203125" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" customWidth="1"/>
+    <col min="12" max="12" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I2" t="s">
+        <v>218</v>
+      </c>
+      <c r="J2" t="s">
+        <v>219</v>
+      </c>
+      <c r="K2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>191</v>
       </c>
-      <c r="B2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" t="s">
         <v>213</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" t="s">
         <v>214</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G3" t="s">
+        <v>216</v>
+      </c>
+      <c r="H3" t="s">
+        <v>224</v>
+      </c>
+      <c r="I3" t="s">
+        <v>218</v>
+      </c>
+      <c r="J3" t="s">
+        <v>219</v>
+      </c>
+      <c r="K3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H4" t="s">
+        <v>227</v>
+      </c>
+      <c r="I4" t="s">
+        <v>218</v>
+      </c>
+      <c r="J4" t="s">
+        <v>219</v>
+      </c>
+      <c r="K4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F5" t="s">
+        <v>231</v>
+      </c>
+      <c r="G5" t="s">
+        <v>216</v>
+      </c>
+      <c r="H5" t="s">
+        <v>232</v>
+      </c>
+      <c r="I5" t="s">
+        <v>218</v>
+      </c>
+      <c r="J5" t="s">
+        <v>219</v>
+      </c>
+      <c r="K5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E6" t="s">
+        <v>235</v>
+      </c>
+      <c r="F6" t="s">
+        <v>223</v>
+      </c>
+      <c r="G6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H6" t="s">
+        <v>236</v>
+      </c>
+      <c r="I6" t="s">
+        <v>218</v>
+      </c>
+      <c r="J6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F7" t="s">
+        <v>223</v>
+      </c>
+      <c r="G7" t="s">
+        <v>216</v>
+      </c>
+      <c r="H7" t="s">
+        <v>240</v>
+      </c>
+      <c r="I7" t="s">
+        <v>218</v>
+      </c>
+      <c r="J7" t="s">
+        <v>219</v>
+      </c>
+      <c r="K7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" t="s">
+        <v>243</v>
+      </c>
+      <c r="F8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G8" t="s">
+        <v>216</v>
+      </c>
+      <c r="H8" t="s">
+        <v>244</v>
+      </c>
+      <c r="I8" t="s">
+        <v>218</v>
+      </c>
+      <c r="J8" t="s">
+        <v>219</v>
+      </c>
+      <c r="K8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" t="s">
+        <v>247</v>
+      </c>
+      <c r="F9" t="s">
+        <v>223</v>
+      </c>
+      <c r="G9" t="s">
+        <v>216</v>
+      </c>
+      <c r="H9" t="s">
+        <v>248</v>
+      </c>
+      <c r="I9" t="s">
+        <v>218</v>
+      </c>
+      <c r="J9" t="s">
+        <v>219</v>
+      </c>
+      <c r="K9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E10" t="s">
+        <v>251</v>
+      </c>
+      <c r="F10" t="s">
         <v>215</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G10" t="s">
         <v>216</v>
       </c>
-      <c r="G2" t="s">
-        <v>217</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="H10" t="s">
+        <v>252</v>
+      </c>
+      <c r="I10" t="s">
         <v>218</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J10" t="s">
         <v>219</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K10" t="s">
         <v>220</v>
       </c>
-      <c r="K2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" t="s">
-        <v>214</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" t="s">
+        <v>255</v>
+      </c>
+      <c r="E11" t="s">
+        <v>256</v>
+      </c>
+      <c r="F11" t="s">
         <v>215</v>
       </c>
-      <c r="F3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G3" t="s">
-        <v>217</v>
-      </c>
-      <c r="H3" t="s">
-        <v>225</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="G11" t="s">
+        <v>216</v>
+      </c>
+      <c r="H11" t="s">
+        <v>257</v>
+      </c>
+      <c r="I11" t="s">
+        <v>218</v>
+      </c>
+      <c r="J11" t="s">
         <v>219</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D12" t="s">
+        <v>255</v>
+      </c>
+      <c r="E12" t="s">
+        <v>260</v>
+      </c>
+      <c r="F12" t="s">
+        <v>261</v>
+      </c>
+      <c r="G12" t="s">
+        <v>216</v>
+      </c>
+      <c r="H12" t="s">
+        <v>262</v>
+      </c>
+      <c r="I12" t="s">
+        <v>218</v>
+      </c>
+      <c r="J12" t="s">
+        <v>219</v>
+      </c>
+      <c r="K12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D13" t="s">
+        <v>255</v>
+      </c>
+      <c r="E13" t="s">
+        <v>265</v>
+      </c>
+      <c r="F13" t="s">
+        <v>215</v>
+      </c>
+      <c r="G13" t="s">
+        <v>216</v>
+      </c>
+      <c r="H13" t="s">
+        <v>266</v>
+      </c>
+      <c r="I13" t="s">
+        <v>218</v>
+      </c>
+      <c r="J13" t="s">
+        <v>219</v>
+      </c>
+      <c r="K13" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" t="s">
+        <v>267</v>
+      </c>
+      <c r="C14" t="s">
+        <v>268</v>
+      </c>
+      <c r="D14" t="s">
+        <v>255</v>
+      </c>
+      <c r="E14" t="s">
+        <v>269</v>
+      </c>
+      <c r="F14" t="s">
+        <v>270</v>
+      </c>
+      <c r="G14" t="s">
+        <v>216</v>
+      </c>
+      <c r="H14" t="s">
+        <v>271</v>
+      </c>
+      <c r="I14" t="s">
+        <v>218</v>
+      </c>
+      <c r="J14" t="s">
+        <v>219</v>
+      </c>
+      <c r="K14" t="s">
         <v>220</v>
       </c>
-      <c r="K3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>193</v>
-      </c>
-      <c r="B4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D4" t="s">
-        <v>214</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" t="s">
+        <v>273</v>
+      </c>
+      <c r="D15" t="s">
+        <v>255</v>
+      </c>
+      <c r="E15" t="s">
+        <v>274</v>
+      </c>
+      <c r="F15" t="s">
         <v>215</v>
       </c>
-      <c r="F4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G4" t="s">
-        <v>217</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G15" t="s">
+        <v>216</v>
+      </c>
+      <c r="H15" t="s">
+        <v>275</v>
+      </c>
+      <c r="I15" t="s">
+        <v>218</v>
+      </c>
+      <c r="J15" t="s">
+        <v>219</v>
+      </c>
+      <c r="K15" t="s">
         <v>228</v>
       </c>
-      <c r="I4" t="s">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B16" t="s">
+        <v>276</v>
+      </c>
+      <c r="C16" t="s">
+        <v>277</v>
+      </c>
+      <c r="D16" t="s">
+        <v>255</v>
+      </c>
+      <c r="E16" t="s">
+        <v>274</v>
+      </c>
+      <c r="F16" t="s">
+        <v>231</v>
+      </c>
+      <c r="G16" t="s">
+        <v>216</v>
+      </c>
+      <c r="H16" t="s">
+        <v>278</v>
+      </c>
+      <c r="I16" t="s">
+        <v>279</v>
+      </c>
+      <c r="J16" t="s">
         <v>219</v>
       </c>
-      <c r="J4" t="s">
-        <v>220</v>
-      </c>
-      <c r="K4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B5" t="s">
-        <v>230</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="K16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17" t="s">
+        <v>280</v>
+      </c>
+      <c r="C17" t="s">
+        <v>281</v>
+      </c>
+      <c r="D17" t="s">
+        <v>255</v>
+      </c>
+      <c r="E17" t="s">
+        <v>282</v>
+      </c>
+      <c r="F17" t="s">
+        <v>261</v>
+      </c>
+      <c r="G17" t="s">
+        <v>216</v>
+      </c>
+      <c r="H17" t="s">
+        <v>283</v>
+      </c>
+      <c r="I17" t="s">
+        <v>218</v>
+      </c>
+      <c r="J17" t="s">
+        <v>219</v>
+      </c>
+      <c r="K17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18" t="s">
+        <v>284</v>
+      </c>
+      <c r="C18" t="s">
+        <v>285</v>
+      </c>
+      <c r="D18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E18" t="s">
+        <v>274</v>
+      </c>
+      <c r="F18" t="s">
+        <v>215</v>
+      </c>
+      <c r="G18" t="s">
+        <v>216</v>
+      </c>
+      <c r="H18" t="s">
+        <v>286</v>
+      </c>
+      <c r="I18" t="s">
+        <v>218</v>
+      </c>
+      <c r="J18" t="s">
+        <v>219</v>
+      </c>
+      <c r="K18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19" t="s">
+        <v>287</v>
+      </c>
+      <c r="C19" t="s">
+        <v>288</v>
+      </c>
+      <c r="D19" t="s">
+        <v>213</v>
+      </c>
+      <c r="E19" t="s">
+        <v>289</v>
+      </c>
+      <c r="F19" t="s">
+        <v>215</v>
+      </c>
+      <c r="G19" t="s">
+        <v>216</v>
+      </c>
+      <c r="H19" t="s">
+        <v>290</v>
+      </c>
+      <c r="I19" t="s">
+        <v>279</v>
+      </c>
+      <c r="J19" t="s">
+        <v>219</v>
+      </c>
+      <c r="K19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B20" t="s">
+        <v>291</v>
+      </c>
+      <c r="C20" t="s">
+        <v>292</v>
+      </c>
+      <c r="D20" t="s">
+        <v>213</v>
+      </c>
+      <c r="E20" t="s">
+        <v>293</v>
+      </c>
+      <c r="F20" t="s">
+        <v>294</v>
+      </c>
+      <c r="G20" t="s">
+        <v>216</v>
+      </c>
+      <c r="H20" t="s">
+        <v>295</v>
+      </c>
+      <c r="I20" t="s">
+        <v>279</v>
+      </c>
+      <c r="J20" t="s">
+        <v>219</v>
+      </c>
+      <c r="K20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>209</v>
+      </c>
+      <c r="B21" t="s">
+        <v>296</v>
+      </c>
+      <c r="C21" t="s">
+        <v>297</v>
+      </c>
+      <c r="D21" t="s">
+        <v>298</v>
+      </c>
+      <c r="E21" t="s">
+        <v>299</v>
+      </c>
+      <c r="F21" t="s">
         <v>231</v>
       </c>
-      <c r="D5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E5" t="s">
-        <v>215</v>
-      </c>
-      <c r="F5" t="s">
-        <v>232</v>
-      </c>
-      <c r="G5" t="s">
-        <v>217</v>
-      </c>
-      <c r="H5" t="s">
-        <v>233</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="G21" t="s">
+        <v>216</v>
+      </c>
+      <c r="H21" t="s">
+        <v>300</v>
+      </c>
+      <c r="I21" t="s">
+        <v>279</v>
+      </c>
+      <c r="J21" t="s">
         <v>219</v>
       </c>
-      <c r="J5" t="s">
-        <v>220</v>
-      </c>
-      <c r="K5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" t="s">
-        <v>234</v>
-      </c>
-      <c r="C6" t="s">
-        <v>235</v>
-      </c>
-      <c r="D6" t="s">
-        <v>214</v>
-      </c>
-      <c r="E6" t="s">
-        <v>236</v>
-      </c>
-      <c r="F6" t="s">
-        <v>224</v>
-      </c>
-      <c r="G6" t="s">
-        <v>217</v>
-      </c>
-      <c r="H6" t="s">
-        <v>237</v>
-      </c>
-      <c r="I6" t="s">
-        <v>219</v>
-      </c>
-      <c r="J6" t="s">
-        <v>220</v>
-      </c>
-      <c r="K6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C7" t="s">
-        <v>239</v>
-      </c>
-      <c r="D7" t="s">
-        <v>214</v>
-      </c>
-      <c r="E7" t="s">
-        <v>240</v>
-      </c>
-      <c r="F7" t="s">
-        <v>224</v>
-      </c>
-      <c r="G7" t="s">
-        <v>217</v>
-      </c>
-      <c r="H7" t="s">
-        <v>241</v>
-      </c>
-      <c r="I7" t="s">
-        <v>219</v>
-      </c>
-      <c r="J7" t="s">
-        <v>220</v>
-      </c>
-      <c r="K7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>197</v>
-      </c>
-      <c r="B8" t="s">
-        <v>242</v>
-      </c>
-      <c r="C8" t="s">
-        <v>243</v>
-      </c>
-      <c r="D8" t="s">
-        <v>214</v>
-      </c>
-      <c r="E8" t="s">
-        <v>244</v>
-      </c>
-      <c r="F8" t="s">
-        <v>224</v>
-      </c>
-      <c r="G8" t="s">
-        <v>217</v>
-      </c>
-      <c r="H8" t="s">
-        <v>245</v>
-      </c>
-      <c r="I8" t="s">
-        <v>219</v>
-      </c>
-      <c r="J8" t="s">
-        <v>220</v>
-      </c>
-      <c r="K8" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>198</v>
-      </c>
-      <c r="B9" t="s">
-        <v>246</v>
-      </c>
-      <c r="C9" t="s">
-        <v>247</v>
-      </c>
-      <c r="D9" t="s">
-        <v>214</v>
-      </c>
-      <c r="E9" t="s">
-        <v>248</v>
-      </c>
-      <c r="F9" t="s">
-        <v>224</v>
-      </c>
-      <c r="G9" t="s">
-        <v>217</v>
-      </c>
-      <c r="H9" t="s">
-        <v>249</v>
-      </c>
-      <c r="I9" t="s">
-        <v>219</v>
-      </c>
-      <c r="J9" t="s">
-        <v>220</v>
-      </c>
-      <c r="K9" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>199</v>
-      </c>
-      <c r="B10" t="s">
-        <v>250</v>
-      </c>
-      <c r="C10" t="s">
-        <v>251</v>
-      </c>
-      <c r="D10" t="s">
-        <v>214</v>
-      </c>
-      <c r="E10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F10" t="s">
-        <v>216</v>
-      </c>
-      <c r="G10" t="s">
-        <v>217</v>
-      </c>
-      <c r="H10" t="s">
-        <v>253</v>
-      </c>
-      <c r="I10" t="s">
-        <v>219</v>
-      </c>
-      <c r="J10" t="s">
-        <v>220</v>
-      </c>
-      <c r="K10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B11" t="s">
-        <v>254</v>
-      </c>
-      <c r="C11" t="s">
-        <v>255</v>
-      </c>
-      <c r="D11" t="s">
-        <v>256</v>
-      </c>
-      <c r="E11" t="s">
-        <v>257</v>
-      </c>
-      <c r="F11" t="s">
-        <v>216</v>
-      </c>
-      <c r="G11" t="s">
-        <v>217</v>
-      </c>
-      <c r="H11" t="s">
-        <v>258</v>
-      </c>
-      <c r="I11" t="s">
-        <v>219</v>
-      </c>
-      <c r="J11" t="s">
-        <v>220</v>
-      </c>
-      <c r="K11" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>201</v>
-      </c>
-      <c r="B12" t="s">
-        <v>259</v>
-      </c>
-      <c r="C12" t="s">
-        <v>260</v>
-      </c>
-      <c r="D12" t="s">
-        <v>256</v>
-      </c>
-      <c r="E12" t="s">
-        <v>261</v>
-      </c>
-      <c r="F12" t="s">
-        <v>262</v>
-      </c>
-      <c r="G12" t="s">
-        <v>217</v>
-      </c>
-      <c r="H12" t="s">
-        <v>263</v>
-      </c>
-      <c r="I12" t="s">
-        <v>219</v>
-      </c>
-      <c r="J12" t="s">
-        <v>220</v>
-      </c>
-      <c r="K12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B13" t="s">
-        <v>264</v>
-      </c>
-      <c r="C13" t="s">
-        <v>265</v>
-      </c>
-      <c r="D13" t="s">
-        <v>256</v>
-      </c>
-      <c r="E13" t="s">
-        <v>266</v>
-      </c>
-      <c r="F13" t="s">
-        <v>216</v>
-      </c>
-      <c r="G13" t="s">
-        <v>217</v>
-      </c>
-      <c r="H13" t="s">
-        <v>267</v>
-      </c>
-      <c r="I13" t="s">
-        <v>219</v>
-      </c>
-      <c r="J13" t="s">
-        <v>220</v>
-      </c>
-      <c r="K13" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>203</v>
-      </c>
-      <c r="B14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C14" t="s">
-        <v>269</v>
-      </c>
-      <c r="D14" t="s">
-        <v>256</v>
-      </c>
-      <c r="E14" t="s">
-        <v>270</v>
-      </c>
-      <c r="F14" t="s">
-        <v>271</v>
-      </c>
-      <c r="G14" t="s">
-        <v>217</v>
-      </c>
-      <c r="H14" t="s">
-        <v>272</v>
-      </c>
-      <c r="I14" t="s">
-        <v>219</v>
-      </c>
-      <c r="J14" t="s">
-        <v>220</v>
-      </c>
-      <c r="K14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>204</v>
-      </c>
-      <c r="B15" t="s">
-        <v>273</v>
-      </c>
-      <c r="C15" t="s">
-        <v>274</v>
-      </c>
-      <c r="D15" t="s">
-        <v>256</v>
-      </c>
-      <c r="E15" t="s">
-        <v>275</v>
-      </c>
-      <c r="F15" t="s">
-        <v>216</v>
-      </c>
-      <c r="G15" t="s">
-        <v>217</v>
-      </c>
-      <c r="H15" t="s">
-        <v>276</v>
-      </c>
-      <c r="I15" t="s">
-        <v>219</v>
-      </c>
-      <c r="J15" t="s">
-        <v>220</v>
-      </c>
-      <c r="K15" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>205</v>
-      </c>
-      <c r="B16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C16" t="s">
-        <v>278</v>
-      </c>
-      <c r="D16" t="s">
-        <v>256</v>
-      </c>
-      <c r="E16" t="s">
-        <v>275</v>
-      </c>
-      <c r="F16" t="s">
-        <v>232</v>
-      </c>
-      <c r="G16" t="s">
-        <v>217</v>
-      </c>
-      <c r="H16" t="s">
-        <v>279</v>
-      </c>
-      <c r="I16" t="s">
-        <v>280</v>
-      </c>
-      <c r="J16" t="s">
-        <v>220</v>
-      </c>
-      <c r="K16" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>206</v>
-      </c>
-      <c r="B17" t="s">
-        <v>281</v>
-      </c>
-      <c r="C17" t="s">
-        <v>282</v>
-      </c>
-      <c r="D17" t="s">
-        <v>256</v>
-      </c>
-      <c r="E17" t="s">
-        <v>283</v>
-      </c>
-      <c r="F17" t="s">
-        <v>262</v>
-      </c>
-      <c r="G17" t="s">
-        <v>217</v>
-      </c>
-      <c r="H17" t="s">
-        <v>284</v>
-      </c>
-      <c r="I17" t="s">
-        <v>219</v>
-      </c>
-      <c r="J17" t="s">
-        <v>220</v>
-      </c>
-      <c r="K17" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>207</v>
-      </c>
-      <c r="B18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C18" t="s">
-        <v>286</v>
-      </c>
-      <c r="D18" t="s">
-        <v>256</v>
-      </c>
-      <c r="E18" t="s">
-        <v>275</v>
-      </c>
-      <c r="F18" t="s">
-        <v>216</v>
-      </c>
-      <c r="G18" t="s">
-        <v>217</v>
-      </c>
-      <c r="H18" t="s">
-        <v>287</v>
-      </c>
-      <c r="I18" t="s">
-        <v>219</v>
-      </c>
-      <c r="J18" t="s">
-        <v>220</v>
-      </c>
-      <c r="K18" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>208</v>
-      </c>
-      <c r="B19" t="s">
-        <v>288</v>
-      </c>
-      <c r="C19" t="s">
-        <v>289</v>
-      </c>
-      <c r="D19" t="s">
-        <v>214</v>
-      </c>
-      <c r="E19" t="s">
-        <v>290</v>
-      </c>
-      <c r="F19" t="s">
-        <v>216</v>
-      </c>
-      <c r="G19" t="s">
-        <v>217</v>
-      </c>
-      <c r="H19" t="s">
-        <v>291</v>
-      </c>
-      <c r="I19" t="s">
-        <v>280</v>
-      </c>
-      <c r="J19" t="s">
-        <v>220</v>
-      </c>
-      <c r="K19" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>209</v>
-      </c>
-      <c r="B20" t="s">
-        <v>292</v>
-      </c>
-      <c r="C20" t="s">
-        <v>293</v>
-      </c>
-      <c r="D20" t="s">
-        <v>214</v>
-      </c>
-      <c r="E20" t="s">
-        <v>294</v>
-      </c>
-      <c r="F20" t="s">
-        <v>295</v>
-      </c>
-      <c r="G20" t="s">
-        <v>217</v>
-      </c>
-      <c r="H20" t="s">
-        <v>296</v>
-      </c>
-      <c r="I20" t="s">
-        <v>280</v>
-      </c>
-      <c r="J20" t="s">
-        <v>220</v>
-      </c>
-      <c r="K20" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>210</v>
-      </c>
-      <c r="B21" t="s">
-        <v>297</v>
-      </c>
-      <c r="C21" t="s">
-        <v>298</v>
-      </c>
-      <c r="D21" t="s">
-        <v>299</v>
-      </c>
-      <c r="E21" t="s">
-        <v>300</v>
-      </c>
-      <c r="F21" t="s">
-        <v>232</v>
-      </c>
-      <c r="G21" t="s">
-        <v>217</v>
-      </c>
-      <c r="H21" t="s">
-        <v>301</v>
-      </c>
-      <c r="I21" t="s">
-        <v>280</v>
-      </c>
-      <c r="J21" t="s">
-        <v>220</v>
-      </c>
       <c r="K21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3842,28 +4112,28 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -3874,7 +4144,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -3885,7 +4155,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -3896,7 +4166,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -3907,14 +4177,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -3925,7 +4195,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -3936,7 +4206,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3947,7 +4217,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -3958,7 +4228,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -3969,12 +4239,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Reworked Sensitive lists and DR Ids sheet
</commit_message>
<xml_diff>
--- a/analysis/Current-Historical-List-Ids.xlsx
+++ b/analysis/Current-Historical-List-Ids.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/new330/IdeaProjects/authoritative-lists/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oco115\PycharmProjects\authoritative-lists\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479D02A1-A103-A34D-B5EC-C0D112356B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5FA8F4-160F-41B1-AD70-62B9F220EBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59580" yWindow="2520" windowWidth="24900" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21900" yWindow="645" windowWidth="28965" windowHeight="18825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Files Summary" sheetId="4" r:id="rId2"/>
-    <sheet name="Doug - Replacement List" sheetId="2" r:id="rId3"/>
-    <sheet name="Metadata" sheetId="5" r:id="rId4"/>
-    <sheet name="DR Ids" sheetId="3" r:id="rId5"/>
+    <sheet name="File Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Doug - Replacement List" sheetId="2" r:id="rId2"/>
+    <sheet name="Metadata" sheetId="5" r:id="rId3"/>
+    <sheet name="DR Ids" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="360">
   <si>
     <t>Sensitive</t>
   </si>
@@ -553,42 +552,18 @@
     <t>Test - Current New DR ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Sensitive </t>
-  </si>
-  <si>
     <t>NSW</t>
   </si>
   <si>
-    <t>Australia (NSW?)</t>
-  </si>
-  <si>
     <t>Additional Taxa</t>
   </si>
   <si>
-    <t>VIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
     <t>No new list</t>
   </si>
   <si>
-    <t>New list but no matching Historical?</t>
-  </si>
-  <si>
-    <t>Matching List</t>
-  </si>
-  <si>
-    <t>Matching List - region doesn't match</t>
-  </si>
-  <si>
-    <t>No new list - region doesn't match</t>
-  </si>
-  <si>
     <t>dr491</t>
   </si>
   <si>
@@ -598,9 +573,6 @@
     <t>Test Current DR ID</t>
   </si>
   <si>
-    <t>Matching List (duplicate sensitive)</t>
-  </si>
-  <si>
     <t>https://lists.ala.org.au/ws/speciesList/dr656</t>
   </si>
   <si>
@@ -1018,9 +990,6 @@
     <t>https://lists.ala.org.au/speciesListItem/list/dr650</t>
   </si>
   <si>
-    <t>dr18759</t>
-  </si>
-  <si>
     <t>https://lists-test.ala.org.au/speciesListItem/list/dr18396</t>
   </si>
   <si>
@@ -1028,13 +997,124 @@
   </si>
   <si>
     <t>https://lists-test.ala.org.au/speciesListItem/list/dr2201</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18711</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18712</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18713</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18714</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18718</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18703</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18735</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18704</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18701</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18705</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18706</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18736</t>
+  </si>
+  <si>
+    <t>Region name is different</t>
+  </si>
+  <si>
+    <t>https://lists-test.ala.org.au/speciesListItem/list/dr492</t>
+  </si>
+  <si>
+    <t>https://lists-test.ala.org.au/speciesListItem/list/dr884</t>
+  </si>
+  <si>
+    <t>https://lists-test.ala.org.au/speciesListItem/list/dr491</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr2627</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr493</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr490</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr467</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr492</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr884</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr491</t>
+  </si>
+  <si>
+    <t>Other Conservation</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr487</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr1782</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr967</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr494</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr7933</t>
+  </si>
+  <si>
+    <t>Birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Sensitive </t>
+  </si>
+  <si>
+    <t>https://lists-test.ala.org.au/speciesListItem/list/dr1782</t>
+  </si>
+  <si>
+    <t>https://lists-test.ala.org.au/speciesListItem/list/dr967</t>
+  </si>
+  <si>
+    <t>Plantae 2014</t>
+  </si>
+  <si>
+    <t>Animalia 2013</t>
+  </si>
+  <si>
+    <t>https://lists-test.ala.org.au/speciesListItem/list/dr487</t>
+  </si>
+  <si>
+    <t>Now classified as Sensitive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1066,22 +1146,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1092,8 +1157,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1118,6 +1220,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1132,7 +1246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1142,11 +1256,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1428,29 +1550,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G24" sqref="G24:G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="54.140625" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1464,13 +1586,16 @@
         <v>172</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1486,8 +1611,11 @@
       <c r="F3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1504,14 +1632,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E5" t="s">
@@ -1521,828 +1649,778 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B15" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="E15" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C16" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C17" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E17" t="s">
         <v>12</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E18" t="s">
         <v>13</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E19" t="s">
         <v>10</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E20" t="s">
         <v>16</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C14" s="1" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C22" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E22" t="s">
         <v>17</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>175</v>
-      </c>
-      <c r="C16" t="s">
-        <v>316</v>
-      </c>
-      <c r="D16" s="4" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" t="s">
+        <v>307</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="F16" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+      <c r="E23" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F23" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C24" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F17" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E24" s="1"/>
+      <c r="G24" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E38" s="18"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>342</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F39" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B41" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="D27" s="13" t="s">
+      <c r="C41" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="E41" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F43" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>174</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F48" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+      <c r="D50" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E50" s="18"/>
+      <c r="G50" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F34" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" t="s">
-        <v>320</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F35" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+      <c r="F56" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C13" r:id="rId1" xr:uid="{6EE0F20C-BD06-4978-B8CD-E66E5C646CF8}"/>
+    <hyperlink ref="C20" r:id="rId1" xr:uid="{6EE0F20C-BD06-4978-B8CD-E66E5C646CF8}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{986401DC-0BF7-4C73-986B-8606D257EF06}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{952BDF74-1025-44CA-B437-CA7A782DEF2C}"/>
-    <hyperlink ref="D13" r:id="rId4" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BA5A33AF-C0B9-4DFE-9F12-7BFDF7D8A911}"/>
-    <hyperlink ref="E16" r:id="rId5" xr:uid="{ECFB10CF-9B59-4B58-9F8C-86B26ED2D1A6}"/>
-    <hyperlink ref="C32" r:id="rId6" xr:uid="{D698F75E-C3A9-2E43-9EF9-D03CAFBC8EA9}"/>
-    <hyperlink ref="C22" r:id="rId7" xr:uid="{4780244B-70BF-9C48-970A-9B52EE257B77}"/>
-    <hyperlink ref="D32" r:id="rId8" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BCC2EF75-48CD-4548-9585-233F9187C820}"/>
-    <hyperlink ref="A21" r:id="rId9" xr:uid="{4A0B836D-E3B0-794C-A4F5-21AA69E861E2}"/>
+    <hyperlink ref="D20" r:id="rId4" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BA5A33AF-C0B9-4DFE-9F12-7BFDF7D8A911}"/>
+    <hyperlink ref="E23" r:id="rId5" xr:uid="{ECFB10CF-9B59-4B58-9F8C-86B26ED2D1A6}"/>
+    <hyperlink ref="C46" r:id="rId6" xr:uid="{D698F75E-C3A9-2E43-9EF9-D03CAFBC8EA9}"/>
+    <hyperlink ref="C29" r:id="rId7" display="https://lists-test.ala.org.au/speciesListItem/list/dr2627" xr:uid="{4780244B-70BF-9C48-970A-9B52EE257B77}"/>
+    <hyperlink ref="D46" r:id="rId8" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BCC2EF75-48CD-4548-9585-233F9187C820}"/>
+    <hyperlink ref="A28" r:id="rId9" xr:uid="{4A0B836D-E3B0-794C-A4F5-21AA69E861E2}"/>
     <hyperlink ref="A2" r:id="rId10" xr:uid="{6FC89B14-CCA6-C244-9CDE-F11F9F1FF7E7}"/>
-    <hyperlink ref="A8" r:id="rId11" xr:uid="{6366CB73-381F-0249-A1E4-038947A0C509}"/>
-    <hyperlink ref="A27" r:id="rId12" xr:uid="{B8D63856-57FE-8C42-8EAD-AECB4BC1FF98}"/>
-    <hyperlink ref="C27" r:id="rId13" xr:uid="{96429AFB-B264-344B-B15E-8F464D602044}"/>
-    <hyperlink ref="C28" r:id="rId14" xr:uid="{31C2BC7F-43DC-0447-95EB-1702F49CA889}"/>
-    <hyperlink ref="C29" r:id="rId15" xr:uid="{5EF5C7C0-C9E6-624F-BF44-A5738449F8BA}"/>
-    <hyperlink ref="C30" r:id="rId16" xr:uid="{9AA0D4E8-104C-FA40-B731-F1AFD127B25C}"/>
-    <hyperlink ref="C31" r:id="rId17" xr:uid="{0AA1FC7B-6EFA-B54C-A968-3E6832124A77}"/>
-    <hyperlink ref="C33" r:id="rId18" xr:uid="{88BF66EA-B4A9-5B40-A7A3-599D95618642}"/>
-    <hyperlink ref="C34" r:id="rId19" xr:uid="{7A14450F-9C85-3C46-891C-D60F0551E9B5}"/>
-    <hyperlink ref="C17" r:id="rId20" xr:uid="{5A2DA5AE-E509-094D-981A-96E4E13B0899}"/>
+    <hyperlink ref="A15" r:id="rId11" xr:uid="{6366CB73-381F-0249-A1E4-038947A0C509}"/>
+    <hyperlink ref="A41" r:id="rId12" xr:uid="{B8D63856-57FE-8C42-8EAD-AECB4BC1FF98}"/>
+    <hyperlink ref="C41" r:id="rId13" xr:uid="{96429AFB-B264-344B-B15E-8F464D602044}"/>
+    <hyperlink ref="C42" r:id="rId14" xr:uid="{31C2BC7F-43DC-0447-95EB-1702F49CA889}"/>
+    <hyperlink ref="C43" r:id="rId15" xr:uid="{5EF5C7C0-C9E6-624F-BF44-A5738449F8BA}"/>
+    <hyperlink ref="C44" r:id="rId16" xr:uid="{9AA0D4E8-104C-FA40-B731-F1AFD127B25C}"/>
+    <hyperlink ref="C45" r:id="rId17" xr:uid="{0AA1FC7B-6EFA-B54C-A968-3E6832124A77}"/>
+    <hyperlink ref="C47" r:id="rId18" xr:uid="{88BF66EA-B4A9-5B40-A7A3-599D95618642}"/>
+    <hyperlink ref="C48" r:id="rId19" xr:uid="{7A14450F-9C85-3C46-891C-D60F0551E9B5}"/>
+    <hyperlink ref="C24" r:id="rId20" xr:uid="{5A2DA5AE-E509-094D-981A-96E4E13B0899}"/>
+    <hyperlink ref="C31" r:id="rId21" display="https://lists-test.ala.org.au/speciesListItem/list/dr490" xr:uid="{E684EDD1-59E8-432F-83AA-222E20CB276C}"/>
+    <hyperlink ref="E29" r:id="rId22" xr:uid="{600763AB-F816-41F1-8049-22570CC11D0B}"/>
+    <hyperlink ref="E30" r:id="rId23" xr:uid="{8B4FF377-6E00-4C40-A026-AC534597AF83}"/>
+    <hyperlink ref="E31" r:id="rId24" xr:uid="{5DCC8A3F-A15F-4D27-9655-D103A175BED4}"/>
+    <hyperlink ref="E39" r:id="rId25" xr:uid="{7A373A1D-1D80-4574-9F0E-6361ADE6EA1B}"/>
+    <hyperlink ref="E41" r:id="rId26" xr:uid="{D774CFC5-AE6A-4609-9ADC-A7D7C699A6EB}"/>
+    <hyperlink ref="E42" r:id="rId27" xr:uid="{007E7E11-1D71-43C4-A264-4660FCB67FAC}"/>
+    <hyperlink ref="E43" r:id="rId28" xr:uid="{42F37AA5-D002-41C0-B5CE-B2C89A43B972}"/>
+    <hyperlink ref="E44" r:id="rId29" xr:uid="{FE56801B-7C8F-41C7-A5B5-35433F8B885F}"/>
+    <hyperlink ref="E45" r:id="rId30" xr:uid="{13D8FFBA-7AD0-4D3F-ADA5-3DA7818D2543}"/>
+    <hyperlink ref="E46" r:id="rId31" xr:uid="{1999C80C-0543-421A-9E09-CE6EC8403DBC}"/>
+    <hyperlink ref="E47" r:id="rId32" xr:uid="{CDEA47CE-620A-46F0-80F6-04AB3B2B19E0}"/>
+    <hyperlink ref="E48" r:id="rId33" xr:uid="{F8B85F77-E546-4150-86A7-B0F301B0C6F3}"/>
+    <hyperlink ref="C11" r:id="rId34" xr:uid="{FE96DD95-E99E-4362-A5D5-4B69BAAB8B58}"/>
+    <hyperlink ref="C12" r:id="rId35" xr:uid="{B3C11E20-1B34-458E-8A79-AABFC15FBBF8}"/>
+    <hyperlink ref="C13" r:id="rId36" xr:uid="{FBABA9A6-5AD3-4585-AACA-D7F375DF505C}"/>
+    <hyperlink ref="C35" r:id="rId37" display="https://lists-test.ala.org.au/speciesListItem/list/dr492" xr:uid="{5ADFD62E-071D-4D50-A9F1-7DD045E02C7D}"/>
+    <hyperlink ref="C36" r:id="rId38" display="https://lists-test.ala.org.au/speciesListItem/list/dr884" xr:uid="{8135FF93-4DC0-49ED-B2EC-9F87EC85B79E}"/>
+    <hyperlink ref="C37" r:id="rId39" display="https://lists-test.ala.org.au/speciesListItem/list/dr491" xr:uid="{0FA25B88-5583-4A34-91A9-8293F79F5C17}"/>
+    <hyperlink ref="C32:C54" r:id="rId40" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{5E1A38EB-C2FC-4CB9-95BD-919CFF22EC41}"/>
+    <hyperlink ref="C32" r:id="rId41" xr:uid="{2A8CE89C-4876-4A29-B6EB-5A9A6FED5677}"/>
+    <hyperlink ref="C33" r:id="rId42" xr:uid="{F58F9C57-D04A-4DFB-A449-5C8B903F4512}"/>
+    <hyperlink ref="C54" r:id="rId43" xr:uid="{A21E7F06-2AF5-4850-985F-BB2E6FD743BB}"/>
+    <hyperlink ref="C56" r:id="rId44" xr:uid="{6471530C-DA5E-43A6-B7BA-36E8172AC848}"/>
+    <hyperlink ref="C34" r:id="rId45" xr:uid="{0A7CD882-4D7D-4020-A769-C978BA913387}"/>
+    <hyperlink ref="C6:C7" r:id="rId46" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{BF20DF31-07E8-4589-A04E-683DB3D80B17}"/>
+    <hyperlink ref="C6" r:id="rId47" xr:uid="{DFF57021-8E37-4EB9-8920-609DB7F6AE09}"/>
+    <hyperlink ref="C7" r:id="rId48" xr:uid="{C3BFA540-211B-4E9C-9972-BC449B59FDE2}"/>
+    <hyperlink ref="C10" r:id="rId49" xr:uid="{81E37A10-CF0F-46D9-B680-4C4E256C7AD9}"/>
+    <hyperlink ref="C9" r:id="rId50" xr:uid="{FAD36ADC-121E-40F4-9EBD-FF89730D257E}"/>
+    <hyperlink ref="C38" r:id="rId51" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{31740A7B-837C-48ED-907C-B518340A560A}"/>
+    <hyperlink ref="E8" r:id="rId52" xr:uid="{9E262E71-4F7D-4CCE-A7C4-371E3CC124B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId53"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F43AB59-C670-488C-8E62-1F8BBF480EBA}">
-  <dimension ref="A1:F26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1"/>
-    <col min="6" max="6" width="44" customWidth="1"/>
-    <col min="7" max="7" width="38.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>138</v>
-      </c>
-      <c r="F6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>143</v>
-      </c>
-      <c r="F11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>135</v>
-      </c>
-      <c r="F17" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>86</v>
-      </c>
-      <c r="F18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>144</v>
-      </c>
-      <c r="F20" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>138</v>
-      </c>
-      <c r="F21" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s">
-        <v>141</v>
-      </c>
-      <c r="F22" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s">
-        <v>140</v>
-      </c>
-      <c r="F23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>139</v>
-      </c>
-      <c r="F24" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009932E9-3BF2-4CEF-AF54-2DFB95D312F2}">
   <dimension ref="A1:M37"/>
   <sheetViews>
@@ -2350,17 +2428,17 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="31.1640625" customWidth="1"/>
-    <col min="8" max="8" width="44.5" customWidth="1"/>
-    <col min="9" max="9" width="27.5" customWidth="1"/>
-    <col min="10" max="10" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
+    <col min="8" max="8" width="44.42578125" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -2401,7 +2479,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -2430,7 +2508,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -2465,7 +2543,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -2497,7 +2575,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -2529,7 +2607,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -2561,7 +2639,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -2593,7 +2671,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -2619,7 +2697,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -2642,7 +2720,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -2665,7 +2743,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -2688,7 +2766,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -2711,7 +2789,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>136</v>
       </c>
@@ -2734,7 +2812,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
@@ -2757,7 +2835,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -2780,7 +2858,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
@@ -2803,7 +2881,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>41</v>
       </c>
@@ -2826,7 +2904,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>142</v>
       </c>
@@ -2849,7 +2927,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
@@ -2872,7 +2950,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -2895,7 +2973,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>146</v>
       </c>
@@ -2918,7 +2996,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>147</v>
       </c>
@@ -2950,7 +3028,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>150</v>
       </c>
@@ -2979,7 +3057,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>151</v>
       </c>
@@ -3002,7 +3080,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
@@ -3025,7 +3103,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>152</v>
       </c>
@@ -3048,7 +3126,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -3071,7 +3149,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>153</v>
       </c>
@@ -3103,7 +3181,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>155</v>
       </c>
@@ -3135,7 +3213,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>156</v>
       </c>
@@ -3161,7 +3239,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>158</v>
       </c>
@@ -3187,7 +3265,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>160</v>
       </c>
@@ -3213,7 +3291,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>161</v>
       </c>
@@ -3239,7 +3317,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>162</v>
       </c>
@@ -3265,7 +3343,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>166</v>
       </c>
@@ -3288,7 +3366,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>167</v>
       </c>
@@ -3311,7 +3389,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>168</v>
       </c>
@@ -3342,7 +3420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E1CD31-ADFA-4968-B027-EE786ACAB43C}">
   <dimension ref="A1:K21"/>
   <sheetViews>
@@ -3350,755 +3428,755 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.1640625" customWidth="1"/>
-    <col min="2" max="2" width="30.5" customWidth="1"/>
-    <col min="3" max="3" width="70.5" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
-    <col min="5" max="5" width="48.83203125" customWidth="1"/>
+    <col min="1" max="1" width="53.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="70.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="9" max="9" width="22.5" customWidth="1"/>
-    <col min="10" max="10" width="24.83203125" customWidth="1"/>
-    <col min="11" max="11" width="22.83203125" customWidth="1"/>
-    <col min="12" max="12" width="24.5" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" t="s">
+        <v>207</v>
+      </c>
+      <c r="H2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="K2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3" t="s">
+        <v>215</v>
+      </c>
+      <c r="I3" t="s">
+        <v>209</v>
+      </c>
+      <c r="J3" t="s">
+        <v>210</v>
+      </c>
+      <c r="K3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F4" t="s">
+        <v>214</v>
+      </c>
+      <c r="G4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H4" t="s">
+        <v>218</v>
+      </c>
+      <c r="I4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J4" t="s">
+        <v>210</v>
+      </c>
+      <c r="K4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H5" t="s">
+        <v>223</v>
+      </c>
+      <c r="I5" t="s">
+        <v>209</v>
+      </c>
+      <c r="J5" t="s">
+        <v>210</v>
+      </c>
+      <c r="K5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F6" t="s">
+        <v>214</v>
+      </c>
+      <c r="G6" t="s">
+        <v>207</v>
+      </c>
+      <c r="H6" t="s">
+        <v>227</v>
+      </c>
+      <c r="I6" t="s">
+        <v>209</v>
+      </c>
+      <c r="J6" t="s">
+        <v>210</v>
+      </c>
+      <c r="K6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7" t="s">
+        <v>230</v>
+      </c>
+      <c r="F7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" t="s">
+        <v>207</v>
+      </c>
+      <c r="H7" t="s">
+        <v>231</v>
+      </c>
+      <c r="I7" t="s">
+        <v>209</v>
+      </c>
+      <c r="J7" t="s">
+        <v>210</v>
+      </c>
+      <c r="K7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E8" t="s">
+        <v>234</v>
+      </c>
+      <c r="F8" t="s">
+        <v>214</v>
+      </c>
+      <c r="G8" t="s">
+        <v>207</v>
+      </c>
+      <c r="H8" t="s">
+        <v>235</v>
+      </c>
+      <c r="I8" t="s">
+        <v>209</v>
+      </c>
+      <c r="J8" t="s">
+        <v>210</v>
+      </c>
+      <c r="K8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" t="s">
+        <v>238</v>
+      </c>
+      <c r="F9" t="s">
+        <v>214</v>
+      </c>
+      <c r="G9" t="s">
+        <v>207</v>
+      </c>
+      <c r="H9" t="s">
+        <v>239</v>
+      </c>
+      <c r="I9" t="s">
+        <v>209</v>
+      </c>
+      <c r="J9" t="s">
+        <v>210</v>
+      </c>
+      <c r="K9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" t="s">
+        <v>241</v>
+      </c>
+      <c r="D10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E10" t="s">
+        <v>242</v>
+      </c>
+      <c r="F10" t="s">
+        <v>206</v>
+      </c>
+      <c r="G10" t="s">
+        <v>207</v>
+      </c>
+      <c r="H10" t="s">
+        <v>243</v>
+      </c>
+      <c r="I10" t="s">
+        <v>209</v>
+      </c>
+      <c r="J10" t="s">
+        <v>210</v>
+      </c>
+      <c r="K10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>190</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C11" t="s">
+        <v>245</v>
+      </c>
+      <c r="D11" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" t="s">
+        <v>206</v>
+      </c>
+      <c r="G11" t="s">
+        <v>207</v>
+      </c>
+      <c r="H11" t="s">
+        <v>248</v>
+      </c>
+      <c r="I11" t="s">
+        <v>209</v>
+      </c>
+      <c r="J11" t="s">
+        <v>210</v>
+      </c>
+      <c r="K11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" t="s">
+        <v>250</v>
+      </c>
+      <c r="D12" t="s">
+        <v>246</v>
+      </c>
+      <c r="E12" t="s">
+        <v>251</v>
+      </c>
+      <c r="F12" t="s">
+        <v>252</v>
+      </c>
+      <c r="G12" t="s">
+        <v>207</v>
+      </c>
+      <c r="H12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I12" t="s">
+        <v>209</v>
+      </c>
+      <c r="J12" t="s">
+        <v>210</v>
+      </c>
+      <c r="K12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C13" t="s">
+        <v>255</v>
+      </c>
+      <c r="D13" t="s">
+        <v>246</v>
+      </c>
+      <c r="E13" t="s">
+        <v>256</v>
+      </c>
+      <c r="F13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G13" t="s">
+        <v>207</v>
+      </c>
+      <c r="H13" t="s">
+        <v>257</v>
+      </c>
+      <c r="I13" t="s">
+        <v>209</v>
+      </c>
+      <c r="J13" t="s">
+        <v>210</v>
+      </c>
+      <c r="K13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" t="s">
+        <v>246</v>
+      </c>
+      <c r="E14" t="s">
+        <v>260</v>
+      </c>
+      <c r="F14" t="s">
+        <v>261</v>
+      </c>
+      <c r="G14" t="s">
+        <v>207</v>
+      </c>
+      <c r="H14" t="s">
+        <v>262</v>
+      </c>
+      <c r="I14" t="s">
+        <v>209</v>
+      </c>
+      <c r="J14" t="s">
+        <v>210</v>
+      </c>
+      <c r="K14" t="s">
         <v>211</v>
       </c>
-      <c r="C2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G2" t="s">
-        <v>216</v>
-      </c>
-      <c r="H2" t="s">
-        <v>217</v>
-      </c>
-      <c r="I2" t="s">
-        <v>218</v>
-      </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C15" t="s">
+        <v>264</v>
+      </c>
+      <c r="D15" t="s">
+        <v>246</v>
+      </c>
+      <c r="E15" t="s">
+        <v>265</v>
+      </c>
+      <c r="F15" t="s">
+        <v>206</v>
+      </c>
+      <c r="G15" t="s">
+        <v>207</v>
+      </c>
+      <c r="H15" t="s">
+        <v>266</v>
+      </c>
+      <c r="I15" t="s">
+        <v>209</v>
+      </c>
+      <c r="J15" t="s">
+        <v>210</v>
+      </c>
+      <c r="K15" t="s">
         <v>219</v>
       </c>
-      <c r="K2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" t="s">
+        <v>267</v>
+      </c>
+      <c r="C16" t="s">
+        <v>268</v>
+      </c>
+      <c r="D16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E16" t="s">
+        <v>265</v>
+      </c>
+      <c r="F16" t="s">
         <v>222</v>
       </c>
-      <c r="D3" t="s">
-        <v>213</v>
-      </c>
-      <c r="E3" t="s">
-        <v>214</v>
-      </c>
-      <c r="F3" t="s">
-        <v>223</v>
-      </c>
-      <c r="G3" t="s">
-        <v>216</v>
-      </c>
-      <c r="H3" t="s">
-        <v>224</v>
-      </c>
-      <c r="I3" t="s">
-        <v>218</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="G16" t="s">
+        <v>207</v>
+      </c>
+      <c r="H16" t="s">
+        <v>269</v>
+      </c>
+      <c r="I16" t="s">
+        <v>270</v>
+      </c>
+      <c r="J16" t="s">
+        <v>210</v>
+      </c>
+      <c r="K16" t="s">
         <v>219</v>
       </c>
-      <c r="K3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" t="s">
-        <v>226</v>
-      </c>
-      <c r="D4" t="s">
-        <v>213</v>
-      </c>
-      <c r="E4" t="s">
-        <v>214</v>
-      </c>
-      <c r="F4" t="s">
-        <v>223</v>
-      </c>
-      <c r="G4" t="s">
-        <v>216</v>
-      </c>
-      <c r="H4" t="s">
-        <v>227</v>
-      </c>
-      <c r="I4" t="s">
-        <v>218</v>
-      </c>
-      <c r="J4" t="s">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" t="s">
+        <v>271</v>
+      </c>
+      <c r="C17" t="s">
+        <v>272</v>
+      </c>
+      <c r="D17" t="s">
+        <v>246</v>
+      </c>
+      <c r="E17" t="s">
+        <v>273</v>
+      </c>
+      <c r="F17" t="s">
+        <v>252</v>
+      </c>
+      <c r="G17" t="s">
+        <v>207</v>
+      </c>
+      <c r="H17" t="s">
+        <v>274</v>
+      </c>
+      <c r="I17" t="s">
+        <v>209</v>
+      </c>
+      <c r="J17" t="s">
+        <v>210</v>
+      </c>
+      <c r="K17" t="s">
         <v>219</v>
       </c>
-      <c r="K4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C5" t="s">
-        <v>230</v>
-      </c>
-      <c r="D5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E5" t="s">
-        <v>214</v>
-      </c>
-      <c r="F5" t="s">
-        <v>231</v>
-      </c>
-      <c r="G5" t="s">
-        <v>216</v>
-      </c>
-      <c r="H5" t="s">
-        <v>232</v>
-      </c>
-      <c r="I5" t="s">
-        <v>218</v>
-      </c>
-      <c r="J5" t="s">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>197</v>
+      </c>
+      <c r="B18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C18" t="s">
+        <v>276</v>
+      </c>
+      <c r="D18" t="s">
+        <v>246</v>
+      </c>
+      <c r="E18" t="s">
+        <v>265</v>
+      </c>
+      <c r="F18" t="s">
+        <v>206</v>
+      </c>
+      <c r="G18" t="s">
+        <v>207</v>
+      </c>
+      <c r="H18" t="s">
+        <v>277</v>
+      </c>
+      <c r="I18" t="s">
+        <v>209</v>
+      </c>
+      <c r="J18" t="s">
+        <v>210</v>
+      </c>
+      <c r="K18" t="s">
         <v>219</v>
       </c>
-      <c r="K5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B6" t="s">
-        <v>233</v>
-      </c>
-      <c r="C6" t="s">
-        <v>234</v>
-      </c>
-      <c r="D6" t="s">
-        <v>213</v>
-      </c>
-      <c r="E6" t="s">
-        <v>235</v>
-      </c>
-      <c r="F6" t="s">
-        <v>223</v>
-      </c>
-      <c r="G6" t="s">
-        <v>216</v>
-      </c>
-      <c r="H6" t="s">
-        <v>236</v>
-      </c>
-      <c r="I6" t="s">
-        <v>218</v>
-      </c>
-      <c r="J6" t="s">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>198</v>
+      </c>
+      <c r="B19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C19" t="s">
+        <v>279</v>
+      </c>
+      <c r="D19" t="s">
+        <v>204</v>
+      </c>
+      <c r="E19" t="s">
+        <v>280</v>
+      </c>
+      <c r="F19" t="s">
+        <v>206</v>
+      </c>
+      <c r="G19" t="s">
+        <v>207</v>
+      </c>
+      <c r="H19" t="s">
+        <v>281</v>
+      </c>
+      <c r="I19" t="s">
+        <v>270</v>
+      </c>
+      <c r="J19" t="s">
+        <v>210</v>
+      </c>
+      <c r="K19" t="s">
         <v>219</v>
       </c>
-      <c r="K6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B7" t="s">
-        <v>237</v>
-      </c>
-      <c r="C7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D7" t="s">
-        <v>213</v>
-      </c>
-      <c r="E7" t="s">
-        <v>239</v>
-      </c>
-      <c r="F7" t="s">
-        <v>223</v>
-      </c>
-      <c r="G7" t="s">
-        <v>216</v>
-      </c>
-      <c r="H7" t="s">
-        <v>240</v>
-      </c>
-      <c r="I7" t="s">
-        <v>218</v>
-      </c>
-      <c r="J7" t="s">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B20" t="s">
+        <v>282</v>
+      </c>
+      <c r="C20" t="s">
+        <v>283</v>
+      </c>
+      <c r="D20" t="s">
+        <v>204</v>
+      </c>
+      <c r="E20" t="s">
+        <v>284</v>
+      </c>
+      <c r="F20" t="s">
+        <v>285</v>
+      </c>
+      <c r="G20" t="s">
+        <v>207</v>
+      </c>
+      <c r="H20" t="s">
+        <v>286</v>
+      </c>
+      <c r="I20" t="s">
+        <v>270</v>
+      </c>
+      <c r="J20" t="s">
+        <v>210</v>
+      </c>
+      <c r="K20" t="s">
         <v>219</v>
       </c>
-      <c r="K7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>196</v>
-      </c>
-      <c r="B8" t="s">
-        <v>241</v>
-      </c>
-      <c r="C8" t="s">
-        <v>242</v>
-      </c>
-      <c r="D8" t="s">
-        <v>213</v>
-      </c>
-      <c r="E8" t="s">
-        <v>243</v>
-      </c>
-      <c r="F8" t="s">
-        <v>223</v>
-      </c>
-      <c r="G8" t="s">
-        <v>216</v>
-      </c>
-      <c r="H8" t="s">
-        <v>244</v>
-      </c>
-      <c r="I8" t="s">
-        <v>218</v>
-      </c>
-      <c r="J8" t="s">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" t="s">
+        <v>287</v>
+      </c>
+      <c r="C21" t="s">
+        <v>288</v>
+      </c>
+      <c r="D21" t="s">
+        <v>289</v>
+      </c>
+      <c r="E21" t="s">
+        <v>290</v>
+      </c>
+      <c r="F21" t="s">
+        <v>222</v>
+      </c>
+      <c r="G21" t="s">
+        <v>207</v>
+      </c>
+      <c r="H21" t="s">
+        <v>291</v>
+      </c>
+      <c r="I21" t="s">
+        <v>270</v>
+      </c>
+      <c r="J21" t="s">
+        <v>210</v>
+      </c>
+      <c r="K21" t="s">
         <v>219</v>
-      </c>
-      <c r="K8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>197</v>
-      </c>
-      <c r="B9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D9" t="s">
-        <v>213</v>
-      </c>
-      <c r="E9" t="s">
-        <v>247</v>
-      </c>
-      <c r="F9" t="s">
-        <v>223</v>
-      </c>
-      <c r="G9" t="s">
-        <v>216</v>
-      </c>
-      <c r="H9" t="s">
-        <v>248</v>
-      </c>
-      <c r="I9" t="s">
-        <v>218</v>
-      </c>
-      <c r="J9" t="s">
-        <v>219</v>
-      </c>
-      <c r="K9" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>198</v>
-      </c>
-      <c r="B10" t="s">
-        <v>249</v>
-      </c>
-      <c r="C10" t="s">
-        <v>250</v>
-      </c>
-      <c r="D10" t="s">
-        <v>213</v>
-      </c>
-      <c r="E10" t="s">
-        <v>251</v>
-      </c>
-      <c r="F10" t="s">
-        <v>215</v>
-      </c>
-      <c r="G10" t="s">
-        <v>216</v>
-      </c>
-      <c r="H10" t="s">
-        <v>252</v>
-      </c>
-      <c r="I10" t="s">
-        <v>218</v>
-      </c>
-      <c r="J10" t="s">
-        <v>219</v>
-      </c>
-      <c r="K10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>199</v>
-      </c>
-      <c r="B11" t="s">
-        <v>253</v>
-      </c>
-      <c r="C11" t="s">
-        <v>254</v>
-      </c>
-      <c r="D11" t="s">
-        <v>255</v>
-      </c>
-      <c r="E11" t="s">
-        <v>256</v>
-      </c>
-      <c r="F11" t="s">
-        <v>215</v>
-      </c>
-      <c r="G11" t="s">
-        <v>216</v>
-      </c>
-      <c r="H11" t="s">
-        <v>257</v>
-      </c>
-      <c r="I11" t="s">
-        <v>218</v>
-      </c>
-      <c r="J11" t="s">
-        <v>219</v>
-      </c>
-      <c r="K11" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>200</v>
-      </c>
-      <c r="B12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D12" t="s">
-        <v>255</v>
-      </c>
-      <c r="E12" t="s">
-        <v>260</v>
-      </c>
-      <c r="F12" t="s">
-        <v>261</v>
-      </c>
-      <c r="G12" t="s">
-        <v>216</v>
-      </c>
-      <c r="H12" t="s">
-        <v>262</v>
-      </c>
-      <c r="I12" t="s">
-        <v>218</v>
-      </c>
-      <c r="J12" t="s">
-        <v>219</v>
-      </c>
-      <c r="K12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>201</v>
-      </c>
-      <c r="B13" t="s">
-        <v>263</v>
-      </c>
-      <c r="C13" t="s">
-        <v>264</v>
-      </c>
-      <c r="D13" t="s">
-        <v>255</v>
-      </c>
-      <c r="E13" t="s">
-        <v>265</v>
-      </c>
-      <c r="F13" t="s">
-        <v>215</v>
-      </c>
-      <c r="G13" t="s">
-        <v>216</v>
-      </c>
-      <c r="H13" t="s">
-        <v>266</v>
-      </c>
-      <c r="I13" t="s">
-        <v>218</v>
-      </c>
-      <c r="J13" t="s">
-        <v>219</v>
-      </c>
-      <c r="K13" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>202</v>
-      </c>
-      <c r="B14" t="s">
-        <v>267</v>
-      </c>
-      <c r="C14" t="s">
-        <v>268</v>
-      </c>
-      <c r="D14" t="s">
-        <v>255</v>
-      </c>
-      <c r="E14" t="s">
-        <v>269</v>
-      </c>
-      <c r="F14" t="s">
-        <v>270</v>
-      </c>
-      <c r="G14" t="s">
-        <v>216</v>
-      </c>
-      <c r="H14" t="s">
-        <v>271</v>
-      </c>
-      <c r="I14" t="s">
-        <v>218</v>
-      </c>
-      <c r="J14" t="s">
-        <v>219</v>
-      </c>
-      <c r="K14" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>203</v>
-      </c>
-      <c r="B15" t="s">
-        <v>272</v>
-      </c>
-      <c r="C15" t="s">
-        <v>273</v>
-      </c>
-      <c r="D15" t="s">
-        <v>255</v>
-      </c>
-      <c r="E15" t="s">
-        <v>274</v>
-      </c>
-      <c r="F15" t="s">
-        <v>215</v>
-      </c>
-      <c r="G15" t="s">
-        <v>216</v>
-      </c>
-      <c r="H15" t="s">
-        <v>275</v>
-      </c>
-      <c r="I15" t="s">
-        <v>218</v>
-      </c>
-      <c r="J15" t="s">
-        <v>219</v>
-      </c>
-      <c r="K15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>204</v>
-      </c>
-      <c r="B16" t="s">
-        <v>276</v>
-      </c>
-      <c r="C16" t="s">
-        <v>277</v>
-      </c>
-      <c r="D16" t="s">
-        <v>255</v>
-      </c>
-      <c r="E16" t="s">
-        <v>274</v>
-      </c>
-      <c r="F16" t="s">
-        <v>231</v>
-      </c>
-      <c r="G16" t="s">
-        <v>216</v>
-      </c>
-      <c r="H16" t="s">
-        <v>278</v>
-      </c>
-      <c r="I16" t="s">
-        <v>279</v>
-      </c>
-      <c r="J16" t="s">
-        <v>219</v>
-      </c>
-      <c r="K16" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>205</v>
-      </c>
-      <c r="B17" t="s">
-        <v>280</v>
-      </c>
-      <c r="C17" t="s">
-        <v>281</v>
-      </c>
-      <c r="D17" t="s">
-        <v>255</v>
-      </c>
-      <c r="E17" t="s">
-        <v>282</v>
-      </c>
-      <c r="F17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G17" t="s">
-        <v>216</v>
-      </c>
-      <c r="H17" t="s">
-        <v>283</v>
-      </c>
-      <c r="I17" t="s">
-        <v>218</v>
-      </c>
-      <c r="J17" t="s">
-        <v>219</v>
-      </c>
-      <c r="K17" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>206</v>
-      </c>
-      <c r="B18" t="s">
-        <v>284</v>
-      </c>
-      <c r="C18" t="s">
-        <v>285</v>
-      </c>
-      <c r="D18" t="s">
-        <v>255</v>
-      </c>
-      <c r="E18" t="s">
-        <v>274</v>
-      </c>
-      <c r="F18" t="s">
-        <v>215</v>
-      </c>
-      <c r="G18" t="s">
-        <v>216</v>
-      </c>
-      <c r="H18" t="s">
-        <v>286</v>
-      </c>
-      <c r="I18" t="s">
-        <v>218</v>
-      </c>
-      <c r="J18" t="s">
-        <v>219</v>
-      </c>
-      <c r="K18" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>207</v>
-      </c>
-      <c r="B19" t="s">
-        <v>287</v>
-      </c>
-      <c r="C19" t="s">
-        <v>288</v>
-      </c>
-      <c r="D19" t="s">
-        <v>213</v>
-      </c>
-      <c r="E19" t="s">
-        <v>289</v>
-      </c>
-      <c r="F19" t="s">
-        <v>215</v>
-      </c>
-      <c r="G19" t="s">
-        <v>216</v>
-      </c>
-      <c r="H19" t="s">
-        <v>290</v>
-      </c>
-      <c r="I19" t="s">
-        <v>279</v>
-      </c>
-      <c r="J19" t="s">
-        <v>219</v>
-      </c>
-      <c r="K19" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>208</v>
-      </c>
-      <c r="B20" t="s">
-        <v>291</v>
-      </c>
-      <c r="C20" t="s">
-        <v>292</v>
-      </c>
-      <c r="D20" t="s">
-        <v>213</v>
-      </c>
-      <c r="E20" t="s">
-        <v>293</v>
-      </c>
-      <c r="F20" t="s">
-        <v>294</v>
-      </c>
-      <c r="G20" t="s">
-        <v>216</v>
-      </c>
-      <c r="H20" t="s">
-        <v>295</v>
-      </c>
-      <c r="I20" t="s">
-        <v>279</v>
-      </c>
-      <c r="J20" t="s">
-        <v>219</v>
-      </c>
-      <c r="K20" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>209</v>
-      </c>
-      <c r="B21" t="s">
-        <v>296</v>
-      </c>
-      <c r="C21" t="s">
-        <v>297</v>
-      </c>
-      <c r="D21" t="s">
-        <v>298</v>
-      </c>
-      <c r="E21" t="s">
-        <v>299</v>
-      </c>
-      <c r="F21" t="s">
-        <v>231</v>
-      </c>
-      <c r="G21" t="s">
-        <v>216</v>
-      </c>
-      <c r="H21" t="s">
-        <v>300</v>
-      </c>
-      <c r="I21" t="s">
-        <v>279</v>
-      </c>
-      <c r="J21" t="s">
-        <v>219</v>
-      </c>
-      <c r="K21" t="s">
-        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -4107,157 +4185,238 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A2CF0A-0BF8-448E-99C2-57F5D470810B}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C10" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D11" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C12" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D12" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C13" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D13" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D14" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D15" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D16" s="8" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A11" r:id="rId1" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{7E9D991E-9148-4379-99B3-DFD1F732DCA6}"/>
+    <hyperlink ref="B15" r:id="rId1" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{517CE8C8-60D2-43EA-919E-915C552D3875}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed references to ACT Sensitive
</commit_message>
<xml_diff>
--- a/analysis/Current-Historical-List-Ids.xlsx
+++ b/analysis/Current-Historical-List-Ids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oco115\PycharmProjects\authoritative-lists\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687777D2-F875-4626-BEEF-1A4BA3D1E965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9F41FD-6434-4515-B5D7-C143325066C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="1800" windowWidth="28890" windowHeight="18825" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3615" yWindow="2850" windowWidth="29925" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="File Summary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="360">
   <si>
     <t>Sensitive</t>
   </si>
@@ -63,9 +63,6 @@
     <t>https://lists-test.ala.org.au/speciesListItem/list/dr18400</t>
   </si>
   <si>
-    <t>https://lists-test.ala.org.au/speciesListItem/list/dr18403</t>
-  </si>
-  <si>
     <t>https://lists-test.ala.org.au/speciesListItem/list/dr18397</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>dr655</t>
   </si>
   <si>
-    <t>dr18403</t>
-  </si>
-  <si>
     <t>dr18404</t>
   </si>
   <si>
@@ -201,9 +195,6 @@
     <t>Prod TMP files</t>
   </si>
   <si>
-    <t>dr18711</t>
-  </si>
-  <si>
     <t>dr18712</t>
   </si>
   <si>
@@ -997,9 +988,6 @@
   </si>
   <si>
     <t>https://lists-test.ala.org.au/speciesListItem/list/dr2201</t>
-  </si>
-  <si>
-    <t>https://lists.ala.org.au/speciesListItem/list/dr18711</t>
   </si>
   <si>
     <t>https://lists.ala.org.au/speciesListItem/list/dr18712</t>
@@ -1564,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,7 +1569,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1592,19 +1580,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1612,19 +1600,14 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>45</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E3" s="1"/>
       <c r="G3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,16 +1615,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1649,16 +1632,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1666,16 +1649,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1683,16 +1666,16 @@
         <v>4</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1700,16 +1683,16 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1717,28 +1700,28 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1746,13 +1729,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1760,47 +1743,47 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1808,16 +1791,16 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1825,16 +1808,16 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1842,16 +1825,16 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1859,16 +1842,16 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1876,27 +1859,27 @@
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1904,33 +1887,33 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C23" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F23" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1938,14 +1921,14 @@
         <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E24" s="1"/>
       <c r="G24" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1953,18 +1936,18 @@
         <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G25" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1975,16 +1958,16 @@
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1992,33 +1975,28 @@
         <v>2</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F29" t="s">
-        <v>57</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2026,16 +2004,16 @@
         <v>4</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2043,16 +2021,16 @@
         <v>4</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2060,33 +2038,33 @@
         <v>4</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2094,13 +2072,13 @@
         <v>7</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2108,27 +2086,27 @@
         <v>8</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2136,10 +2114,10 @@
         <v>5</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E38" s="18"/>
     </row>
@@ -2148,36 +2126,36 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F39" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2185,16 +2163,16 @@
         <v>3</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F42" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2202,16 +2180,16 @@
         <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F43" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2219,16 +2197,16 @@
         <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F44" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2236,16 +2214,16 @@
         <v>8</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F45" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2253,16 +2231,16 @@
         <v>9</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F46" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2270,33 +2248,33 @@
         <v>4</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F47" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F48" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2304,13 +2282,13 @@
         <v>5</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="50" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2318,125 +2296,123 @@
         <v>5</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E50" s="18"/>
       <c r="G50" s="8" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="54" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C20" r:id="rId1" xr:uid="{6EE0F20C-BD06-4978-B8CD-E66E5C646CF8}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{986401DC-0BF7-4C73-986B-8606D257EF06}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{952BDF74-1025-44CA-B437-CA7A782DEF2C}"/>
-    <hyperlink ref="D20" r:id="rId4" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BA5A33AF-C0B9-4DFE-9F12-7BFDF7D8A911}"/>
-    <hyperlink ref="E23" r:id="rId5" xr:uid="{ECFB10CF-9B59-4B58-9F8C-86B26ED2D1A6}"/>
-    <hyperlink ref="C46" r:id="rId6" xr:uid="{D698F75E-C3A9-2E43-9EF9-D03CAFBC8EA9}"/>
-    <hyperlink ref="C29" r:id="rId7" display="https://lists-test.ala.org.au/speciesListItem/list/dr2627" xr:uid="{4780244B-70BF-9C48-970A-9B52EE257B77}"/>
-    <hyperlink ref="D46" r:id="rId8" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BCC2EF75-48CD-4548-9585-233F9187C820}"/>
-    <hyperlink ref="A28" r:id="rId9" xr:uid="{4A0B836D-E3B0-794C-A4F5-21AA69E861E2}"/>
-    <hyperlink ref="A2" r:id="rId10" xr:uid="{6FC89B14-CCA6-C244-9CDE-F11F9F1FF7E7}"/>
-    <hyperlink ref="A15" r:id="rId11" xr:uid="{6366CB73-381F-0249-A1E4-038947A0C509}"/>
-    <hyperlink ref="A41" r:id="rId12" xr:uid="{B8D63856-57FE-8C42-8EAD-AECB4BC1FF98}"/>
-    <hyperlink ref="C41" r:id="rId13" xr:uid="{96429AFB-B264-344B-B15E-8F464D602044}"/>
-    <hyperlink ref="C42" r:id="rId14" xr:uid="{31C2BC7F-43DC-0447-95EB-1702F49CA889}"/>
-    <hyperlink ref="C43" r:id="rId15" xr:uid="{5EF5C7C0-C9E6-624F-BF44-A5738449F8BA}"/>
-    <hyperlink ref="C44" r:id="rId16" xr:uid="{9AA0D4E8-104C-FA40-B731-F1AFD127B25C}"/>
-    <hyperlink ref="C45" r:id="rId17" xr:uid="{0AA1FC7B-6EFA-B54C-A968-3E6832124A77}"/>
-    <hyperlink ref="C47" r:id="rId18" xr:uid="{88BF66EA-B4A9-5B40-A7A3-599D95618642}"/>
-    <hyperlink ref="C48" r:id="rId19" xr:uid="{7A14450F-9C85-3C46-891C-D60F0551E9B5}"/>
-    <hyperlink ref="C24" r:id="rId20" xr:uid="{5A2DA5AE-E509-094D-981A-96E4E13B0899}"/>
-    <hyperlink ref="C31" r:id="rId21" display="https://lists-test.ala.org.au/speciesListItem/list/dr490" xr:uid="{E684EDD1-59E8-432F-83AA-222E20CB276C}"/>
-    <hyperlink ref="E29" r:id="rId22" xr:uid="{600763AB-F816-41F1-8049-22570CC11D0B}"/>
-    <hyperlink ref="E30" r:id="rId23" xr:uid="{8B4FF377-6E00-4C40-A026-AC534597AF83}"/>
-    <hyperlink ref="E31" r:id="rId24" xr:uid="{5DCC8A3F-A15F-4D27-9655-D103A175BED4}"/>
-    <hyperlink ref="E39" r:id="rId25" xr:uid="{7A373A1D-1D80-4574-9F0E-6361ADE6EA1B}"/>
-    <hyperlink ref="E41" r:id="rId26" xr:uid="{D774CFC5-AE6A-4609-9ADC-A7D7C699A6EB}"/>
-    <hyperlink ref="E42" r:id="rId27" xr:uid="{007E7E11-1D71-43C4-A264-4660FCB67FAC}"/>
-    <hyperlink ref="E43" r:id="rId28" xr:uid="{42F37AA5-D002-41C0-B5CE-B2C89A43B972}"/>
-    <hyperlink ref="E44" r:id="rId29" xr:uid="{FE56801B-7C8F-41C7-A5B5-35433F8B885F}"/>
-    <hyperlink ref="E45" r:id="rId30" xr:uid="{13D8FFBA-7AD0-4D3F-ADA5-3DA7818D2543}"/>
-    <hyperlink ref="E46" r:id="rId31" xr:uid="{1999C80C-0543-421A-9E09-CE6EC8403DBC}"/>
-    <hyperlink ref="E47" r:id="rId32" xr:uid="{CDEA47CE-620A-46F0-80F6-04AB3B2B19E0}"/>
-    <hyperlink ref="E48" r:id="rId33" xr:uid="{F8B85F77-E546-4150-86A7-B0F301B0C6F3}"/>
-    <hyperlink ref="C11" r:id="rId34" xr:uid="{FE96DD95-E99E-4362-A5D5-4B69BAAB8B58}"/>
-    <hyperlink ref="C12" r:id="rId35" xr:uid="{B3C11E20-1B34-458E-8A79-AABFC15FBBF8}"/>
-    <hyperlink ref="C13" r:id="rId36" xr:uid="{FBABA9A6-5AD3-4585-AACA-D7F375DF505C}"/>
-    <hyperlink ref="C35" r:id="rId37" display="https://lists-test.ala.org.au/speciesListItem/list/dr492" xr:uid="{5ADFD62E-071D-4D50-A9F1-7DD045E02C7D}"/>
-    <hyperlink ref="C36" r:id="rId38" display="https://lists-test.ala.org.au/speciesListItem/list/dr884" xr:uid="{8135FF93-4DC0-49ED-B2EC-9F87EC85B79E}"/>
-    <hyperlink ref="C37" r:id="rId39" display="https://lists-test.ala.org.au/speciesListItem/list/dr491" xr:uid="{0FA25B88-5583-4A34-91A9-8293F79F5C17}"/>
-    <hyperlink ref="C32:C54" r:id="rId40" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{5E1A38EB-C2FC-4CB9-95BD-919CFF22EC41}"/>
-    <hyperlink ref="C32" r:id="rId41" xr:uid="{2A8CE89C-4876-4A29-B6EB-5A9A6FED5677}"/>
-    <hyperlink ref="C33" r:id="rId42" xr:uid="{F58F9C57-D04A-4DFB-A449-5C8B903F4512}"/>
-    <hyperlink ref="C54" r:id="rId43" xr:uid="{A21E7F06-2AF5-4850-985F-BB2E6FD743BB}"/>
-    <hyperlink ref="C56" r:id="rId44" xr:uid="{6471530C-DA5E-43A6-B7BA-36E8172AC848}"/>
-    <hyperlink ref="C34" r:id="rId45" xr:uid="{0A7CD882-4D7D-4020-A769-C978BA913387}"/>
-    <hyperlink ref="C6:C7" r:id="rId46" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{BF20DF31-07E8-4589-A04E-683DB3D80B17}"/>
-    <hyperlink ref="C6" r:id="rId47" xr:uid="{DFF57021-8E37-4EB9-8920-609DB7F6AE09}"/>
-    <hyperlink ref="C7" r:id="rId48" xr:uid="{C3BFA540-211B-4E9C-9972-BC449B59FDE2}"/>
-    <hyperlink ref="C10" r:id="rId49" xr:uid="{81E37A10-CF0F-46D9-B680-4C4E256C7AD9}"/>
-    <hyperlink ref="C9" r:id="rId50" xr:uid="{FAD36ADC-121E-40F4-9EBD-FF89730D257E}"/>
-    <hyperlink ref="C38" r:id="rId51" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{31740A7B-837C-48ED-907C-B518340A560A}"/>
-    <hyperlink ref="E8" r:id="rId52" xr:uid="{9E262E71-4F7D-4CCE-A7C4-371E3CC124B6}"/>
-    <hyperlink ref="E34" r:id="rId53" xr:uid="{C2D49F08-150A-46F1-B8D5-876F1ACE8778}"/>
-    <hyperlink ref="E10" r:id="rId54" xr:uid="{8D5650F4-48BD-465C-881F-2A05C01FAB4D}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{952BDF74-1025-44CA-B437-CA7A782DEF2C}"/>
+    <hyperlink ref="D20" r:id="rId3" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BA5A33AF-C0B9-4DFE-9F12-7BFDF7D8A911}"/>
+    <hyperlink ref="E23" r:id="rId4" xr:uid="{ECFB10CF-9B59-4B58-9F8C-86B26ED2D1A6}"/>
+    <hyperlink ref="C46" r:id="rId5" xr:uid="{D698F75E-C3A9-2E43-9EF9-D03CAFBC8EA9}"/>
+    <hyperlink ref="C29" r:id="rId6" display="https://lists-test.ala.org.au/speciesListItem/list/dr2627" xr:uid="{4780244B-70BF-9C48-970A-9B52EE257B77}"/>
+    <hyperlink ref="D46" r:id="rId7" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BCC2EF75-48CD-4548-9585-233F9187C820}"/>
+    <hyperlink ref="A28" r:id="rId8" xr:uid="{4A0B836D-E3B0-794C-A4F5-21AA69E861E2}"/>
+    <hyperlink ref="A2" r:id="rId9" xr:uid="{6FC89B14-CCA6-C244-9CDE-F11F9F1FF7E7}"/>
+    <hyperlink ref="A15" r:id="rId10" xr:uid="{6366CB73-381F-0249-A1E4-038947A0C509}"/>
+    <hyperlink ref="A41" r:id="rId11" xr:uid="{B8D63856-57FE-8C42-8EAD-AECB4BC1FF98}"/>
+    <hyperlink ref="C41" r:id="rId12" xr:uid="{96429AFB-B264-344B-B15E-8F464D602044}"/>
+    <hyperlink ref="C42" r:id="rId13" xr:uid="{31C2BC7F-43DC-0447-95EB-1702F49CA889}"/>
+    <hyperlink ref="C43" r:id="rId14" xr:uid="{5EF5C7C0-C9E6-624F-BF44-A5738449F8BA}"/>
+    <hyperlink ref="C44" r:id="rId15" xr:uid="{9AA0D4E8-104C-FA40-B731-F1AFD127B25C}"/>
+    <hyperlink ref="C45" r:id="rId16" xr:uid="{0AA1FC7B-6EFA-B54C-A968-3E6832124A77}"/>
+    <hyperlink ref="C47" r:id="rId17" xr:uid="{88BF66EA-B4A9-5B40-A7A3-599D95618642}"/>
+    <hyperlink ref="C48" r:id="rId18" xr:uid="{7A14450F-9C85-3C46-891C-D60F0551E9B5}"/>
+    <hyperlink ref="C24" r:id="rId19" xr:uid="{5A2DA5AE-E509-094D-981A-96E4E13B0899}"/>
+    <hyperlink ref="C31" r:id="rId20" display="https://lists-test.ala.org.au/speciesListItem/list/dr490" xr:uid="{E684EDD1-59E8-432F-83AA-222E20CB276C}"/>
+    <hyperlink ref="E30" r:id="rId21" xr:uid="{8B4FF377-6E00-4C40-A026-AC534597AF83}"/>
+    <hyperlink ref="E31" r:id="rId22" xr:uid="{5DCC8A3F-A15F-4D27-9655-D103A175BED4}"/>
+    <hyperlink ref="E39" r:id="rId23" xr:uid="{7A373A1D-1D80-4574-9F0E-6361ADE6EA1B}"/>
+    <hyperlink ref="E41" r:id="rId24" xr:uid="{D774CFC5-AE6A-4609-9ADC-A7D7C699A6EB}"/>
+    <hyperlink ref="E42" r:id="rId25" xr:uid="{007E7E11-1D71-43C4-A264-4660FCB67FAC}"/>
+    <hyperlink ref="E43" r:id="rId26" xr:uid="{42F37AA5-D002-41C0-B5CE-B2C89A43B972}"/>
+    <hyperlink ref="E44" r:id="rId27" xr:uid="{FE56801B-7C8F-41C7-A5B5-35433F8B885F}"/>
+    <hyperlink ref="E45" r:id="rId28" xr:uid="{13D8FFBA-7AD0-4D3F-ADA5-3DA7818D2543}"/>
+    <hyperlink ref="E46" r:id="rId29" xr:uid="{1999C80C-0543-421A-9E09-CE6EC8403DBC}"/>
+    <hyperlink ref="E47" r:id="rId30" xr:uid="{CDEA47CE-620A-46F0-80F6-04AB3B2B19E0}"/>
+    <hyperlink ref="E48" r:id="rId31" xr:uid="{F8B85F77-E546-4150-86A7-B0F301B0C6F3}"/>
+    <hyperlink ref="C11" r:id="rId32" xr:uid="{FE96DD95-E99E-4362-A5D5-4B69BAAB8B58}"/>
+    <hyperlink ref="C12" r:id="rId33" xr:uid="{B3C11E20-1B34-458E-8A79-AABFC15FBBF8}"/>
+    <hyperlink ref="C13" r:id="rId34" xr:uid="{FBABA9A6-5AD3-4585-AACA-D7F375DF505C}"/>
+    <hyperlink ref="C35" r:id="rId35" display="https://lists-test.ala.org.au/speciesListItem/list/dr492" xr:uid="{5ADFD62E-071D-4D50-A9F1-7DD045E02C7D}"/>
+    <hyperlink ref="C36" r:id="rId36" display="https://lists-test.ala.org.au/speciesListItem/list/dr884" xr:uid="{8135FF93-4DC0-49ED-B2EC-9F87EC85B79E}"/>
+    <hyperlink ref="C37" r:id="rId37" display="https://lists-test.ala.org.au/speciesListItem/list/dr491" xr:uid="{0FA25B88-5583-4A34-91A9-8293F79F5C17}"/>
+    <hyperlink ref="C32:C54" r:id="rId38" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{5E1A38EB-C2FC-4CB9-95BD-919CFF22EC41}"/>
+    <hyperlink ref="C32" r:id="rId39" xr:uid="{2A8CE89C-4876-4A29-B6EB-5A9A6FED5677}"/>
+    <hyperlink ref="C33" r:id="rId40" xr:uid="{F58F9C57-D04A-4DFB-A449-5C8B903F4512}"/>
+    <hyperlink ref="C54" r:id="rId41" xr:uid="{A21E7F06-2AF5-4850-985F-BB2E6FD743BB}"/>
+    <hyperlink ref="C56" r:id="rId42" xr:uid="{6471530C-DA5E-43A6-B7BA-36E8172AC848}"/>
+    <hyperlink ref="C34" r:id="rId43" xr:uid="{0A7CD882-4D7D-4020-A769-C978BA913387}"/>
+    <hyperlink ref="C6:C7" r:id="rId44" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{BF20DF31-07E8-4589-A04E-683DB3D80B17}"/>
+    <hyperlink ref="C6" r:id="rId45" xr:uid="{DFF57021-8E37-4EB9-8920-609DB7F6AE09}"/>
+    <hyperlink ref="C7" r:id="rId46" xr:uid="{C3BFA540-211B-4E9C-9972-BC449B59FDE2}"/>
+    <hyperlink ref="C10" r:id="rId47" xr:uid="{81E37A10-CF0F-46D9-B680-4C4E256C7AD9}"/>
+    <hyperlink ref="C9" r:id="rId48" xr:uid="{FAD36ADC-121E-40F4-9EBD-FF89730D257E}"/>
+    <hyperlink ref="C38" r:id="rId49" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{31740A7B-837C-48ED-907C-B518340A560A}"/>
+    <hyperlink ref="E8" r:id="rId50" xr:uid="{9E262E71-4F7D-4CCE-A7C4-371E3CC124B6}"/>
+    <hyperlink ref="E34" r:id="rId51" xr:uid="{C2D49F08-150A-46F1-B8D5-876F1ACE8778}"/>
+    <hyperlink ref="E10" r:id="rId52" xr:uid="{8D5650F4-48BD-465C-881F-2A05C01FAB4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId55"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId53"/>
 </worksheet>
 </file>
 
@@ -2460,979 +2436,979 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>77</v>
-      </c>
-      <c r="K1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
         <v>81</v>
       </c>
-      <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>82</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>83</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>84</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
         <v>85</v>
-      </c>
-      <c r="I2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" t="s">
-        <v>87</v>
-      </c>
-      <c r="M2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
         <v>89</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>91</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>92</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" t="s">
         <v>93</v>
       </c>
-      <c r="F3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
         <v>85</v>
-      </c>
-      <c r="I3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J3" t="s">
-        <v>96</v>
-      </c>
-      <c r="M3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
         <v>97</v>
       </c>
-      <c r="B4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>92</v>
       </c>
-      <c r="E4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4" t="s">
-        <v>95</v>
-      </c>
       <c r="H4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" t="s">
         <v>85</v>
-      </c>
-      <c r="I4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" t="s">
-        <v>96</v>
-      </c>
-      <c r="M4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" t="s">
         <v>101</v>
       </c>
-      <c r="B5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" t="s">
         <v>102</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" t="s">
         <v>103</v>
       </c>
-      <c r="F5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J5" t="s">
-        <v>106</v>
-      </c>
       <c r="M5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" t="s">
         <v>107</v>
       </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" t="s">
         <v>108</v>
       </c>
-      <c r="E6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H6" t="s">
-        <v>105</v>
-      </c>
-      <c r="I6" t="s">
-        <v>86</v>
-      </c>
-      <c r="J6" t="s">
-        <v>111</v>
-      </c>
       <c r="M6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" t="s">
         <v>112</v>
       </c>
-      <c r="B7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" t="s">
         <v>113</v>
       </c>
-      <c r="E7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G7" t="s">
-        <v>95</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="M7" t="s">
         <v>85</v>
-      </c>
-      <c r="I7" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" t="s">
-        <v>116</v>
-      </c>
-      <c r="M7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" t="s">
         <v>117</v>
       </c>
-      <c r="B8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="I8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" t="s">
         <v>118</v>
       </c>
-      <c r="F8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K8" t="s">
-        <v>121</v>
-      </c>
       <c r="M8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" t="s">
         <v>122</v>
       </c>
-      <c r="B9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="I9" t="s">
         <v>123</v>
       </c>
-      <c r="F9" t="s">
-        <v>124</v>
-      </c>
-      <c r="H9" t="s">
-        <v>125</v>
-      </c>
-      <c r="I9" t="s">
-        <v>126</v>
-      </c>
       <c r="M9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" t="s">
         <v>127</v>
       </c>
-      <c r="B10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="J10" t="s">
         <v>128</v>
       </c>
-      <c r="F10" t="s">
-        <v>129</v>
-      </c>
-      <c r="H10" t="s">
-        <v>130</v>
-      </c>
-      <c r="J10" t="s">
-        <v>131</v>
-      </c>
       <c r="M10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="L12" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="J29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="L29" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L34" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>165</v>
-      </c>
       <c r="M34" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>166</v>
-      </c>
       <c r="F35" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B37" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C37" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F37" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H37" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I37" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L37" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3466,737 +3442,737 @@
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2" t="s">
         <v>202</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>203</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>204</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>205</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>206</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>207</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>208</v>
-      </c>
-      <c r="I2" t="s">
-        <v>209</v>
-      </c>
-      <c r="J2" t="s">
-        <v>210</v>
-      </c>
-      <c r="K2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3" t="s">
         <v>212</v>
       </c>
-      <c r="C3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D3" t="s">
-        <v>204</v>
-      </c>
-      <c r="E3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F3" t="s">
-        <v>214</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J3" t="s">
         <v>207</v>
       </c>
-      <c r="H3" t="s">
-        <v>215</v>
-      </c>
-      <c r="I3" t="s">
-        <v>209</v>
-      </c>
-      <c r="J3" t="s">
-        <v>210</v>
-      </c>
       <c r="K3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" t="s">
+        <v>215</v>
+      </c>
+      <c r="I4" t="s">
+        <v>206</v>
+      </c>
+      <c r="J4" t="s">
+        <v>207</v>
+      </c>
+      <c r="K4" t="s">
         <v>216</v>
-      </c>
-      <c r="C4" t="s">
-        <v>217</v>
-      </c>
-      <c r="D4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E4" t="s">
-        <v>205</v>
-      </c>
-      <c r="F4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G4" t="s">
-        <v>207</v>
-      </c>
-      <c r="H4" t="s">
-        <v>218</v>
-      </c>
-      <c r="I4" t="s">
-        <v>209</v>
-      </c>
-      <c r="J4" t="s">
-        <v>210</v>
-      </c>
-      <c r="K4" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G5" t="s">
+        <v>204</v>
+      </c>
+      <c r="H5" t="s">
         <v>220</v>
       </c>
-      <c r="C5" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E5" t="s">
-        <v>205</v>
-      </c>
-      <c r="F5" t="s">
-        <v>222</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
+        <v>206</v>
+      </c>
+      <c r="J5" t="s">
         <v>207</v>
       </c>
-      <c r="H5" t="s">
-        <v>223</v>
-      </c>
-      <c r="I5" t="s">
-        <v>209</v>
-      </c>
-      <c r="J5" t="s">
-        <v>210</v>
-      </c>
       <c r="K5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H6" t="s">
         <v>224</v>
       </c>
-      <c r="C6" t="s">
-        <v>225</v>
-      </c>
-      <c r="D6" t="s">
-        <v>204</v>
-      </c>
-      <c r="E6" t="s">
-        <v>226</v>
-      </c>
-      <c r="F6" t="s">
-        <v>214</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J6" t="s">
         <v>207</v>
       </c>
-      <c r="H6" t="s">
-        <v>227</v>
-      </c>
-      <c r="I6" t="s">
-        <v>209</v>
-      </c>
-      <c r="J6" t="s">
-        <v>210</v>
-      </c>
       <c r="K6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" t="s">
         <v>228</v>
       </c>
-      <c r="C7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D7" t="s">
-        <v>204</v>
-      </c>
-      <c r="E7" t="s">
-        <v>230</v>
-      </c>
-      <c r="F7" t="s">
-        <v>214</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J7" t="s">
         <v>207</v>
       </c>
-      <c r="H7" t="s">
-        <v>231</v>
-      </c>
-      <c r="I7" t="s">
-        <v>209</v>
-      </c>
-      <c r="J7" t="s">
-        <v>210</v>
-      </c>
       <c r="K7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8" t="s">
+        <v>231</v>
+      </c>
+      <c r="F8" t="s">
+        <v>211</v>
+      </c>
+      <c r="G8" t="s">
+        <v>204</v>
+      </c>
+      <c r="H8" t="s">
         <v>232</v>
       </c>
-      <c r="C8" t="s">
-        <v>233</v>
-      </c>
-      <c r="D8" t="s">
-        <v>204</v>
-      </c>
-      <c r="E8" t="s">
-        <v>234</v>
-      </c>
-      <c r="F8" t="s">
-        <v>214</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J8" t="s">
         <v>207</v>
       </c>
-      <c r="H8" t="s">
-        <v>235</v>
-      </c>
-      <c r="I8" t="s">
-        <v>209</v>
-      </c>
-      <c r="J8" t="s">
-        <v>210</v>
-      </c>
       <c r="K8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F9" t="s">
+        <v>211</v>
+      </c>
+      <c r="G9" t="s">
+        <v>204</v>
+      </c>
+      <c r="H9" t="s">
         <v>236</v>
       </c>
-      <c r="C9" t="s">
-        <v>237</v>
-      </c>
-      <c r="D9" t="s">
-        <v>204</v>
-      </c>
-      <c r="E9" t="s">
-        <v>238</v>
-      </c>
-      <c r="F9" t="s">
-        <v>214</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
+        <v>206</v>
+      </c>
+      <c r="J9" t="s">
         <v>207</v>
       </c>
-      <c r="H9" t="s">
-        <v>239</v>
-      </c>
-      <c r="I9" t="s">
-        <v>209</v>
-      </c>
-      <c r="J9" t="s">
-        <v>210</v>
-      </c>
       <c r="K9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" t="s">
+        <v>201</v>
+      </c>
+      <c r="E10" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" t="s">
+        <v>203</v>
+      </c>
+      <c r="G10" t="s">
+        <v>204</v>
+      </c>
+      <c r="H10" t="s">
         <v>240</v>
       </c>
-      <c r="C10" t="s">
-        <v>241</v>
-      </c>
-      <c r="D10" t="s">
-        <v>204</v>
-      </c>
-      <c r="E10" t="s">
-        <v>242</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>206</v>
       </c>
-      <c r="G10" t="s">
+      <c r="J10" t="s">
         <v>207</v>
       </c>
-      <c r="H10" t="s">
-        <v>243</v>
-      </c>
-      <c r="I10" t="s">
-        <v>209</v>
-      </c>
-      <c r="J10" t="s">
-        <v>210</v>
-      </c>
       <c r="K10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" t="s">
+        <v>242</v>
+      </c>
+      <c r="D11" t="s">
+        <v>243</v>
+      </c>
+      <c r="E11" t="s">
         <v>244</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
+        <v>203</v>
+      </c>
+      <c r="G11" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" t="s">
         <v>245</v>
       </c>
-      <c r="D11" t="s">
-        <v>246</v>
-      </c>
-      <c r="E11" t="s">
-        <v>247</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="I11" t="s">
         <v>206</v>
       </c>
-      <c r="G11" t="s">
+      <c r="J11" t="s">
         <v>207</v>
       </c>
-      <c r="H11" t="s">
-        <v>248</v>
-      </c>
-      <c r="I11" t="s">
-        <v>209</v>
-      </c>
-      <c r="J11" t="s">
-        <v>210</v>
-      </c>
       <c r="K11" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s">
+        <v>246</v>
+      </c>
+      <c r="C12" t="s">
+        <v>247</v>
+      </c>
+      <c r="D12" t="s">
+        <v>243</v>
+      </c>
+      <c r="E12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F12" t="s">
         <v>249</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G12" t="s">
+        <v>204</v>
+      </c>
+      <c r="H12" t="s">
         <v>250</v>
       </c>
-      <c r="D12" t="s">
-        <v>246</v>
-      </c>
-      <c r="E12" t="s">
-        <v>251</v>
-      </c>
-      <c r="F12" t="s">
-        <v>252</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
+        <v>206</v>
+      </c>
+      <c r="J12" t="s">
         <v>207</v>
       </c>
-      <c r="H12" t="s">
-        <v>253</v>
-      </c>
-      <c r="I12" t="s">
-        <v>209</v>
-      </c>
-      <c r="J12" t="s">
-        <v>210</v>
-      </c>
       <c r="K12" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B13" t="s">
+        <v>251</v>
+      </c>
+      <c r="C13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D13" t="s">
+        <v>243</v>
+      </c>
+      <c r="E13" t="s">
+        <v>253</v>
+      </c>
+      <c r="F13" t="s">
+        <v>203</v>
+      </c>
+      <c r="G13" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" t="s">
         <v>254</v>
       </c>
-      <c r="C13" t="s">
-        <v>255</v>
-      </c>
-      <c r="D13" t="s">
-        <v>246</v>
-      </c>
-      <c r="E13" t="s">
-        <v>256</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="I13" t="s">
         <v>206</v>
       </c>
-      <c r="G13" t="s">
+      <c r="J13" t="s">
         <v>207</v>
       </c>
-      <c r="H13" t="s">
-        <v>257</v>
-      </c>
-      <c r="I13" t="s">
-        <v>209</v>
-      </c>
-      <c r="J13" t="s">
-        <v>210</v>
-      </c>
       <c r="K13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B14" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" t="s">
+        <v>256</v>
+      </c>
+      <c r="D14" t="s">
+        <v>243</v>
+      </c>
+      <c r="E14" t="s">
+        <v>257</v>
+      </c>
+      <c r="F14" t="s">
         <v>258</v>
       </c>
-      <c r="C14" t="s">
+      <c r="G14" t="s">
+        <v>204</v>
+      </c>
+      <c r="H14" t="s">
         <v>259</v>
       </c>
-      <c r="D14" t="s">
-        <v>246</v>
-      </c>
-      <c r="E14" t="s">
-        <v>260</v>
-      </c>
-      <c r="F14" t="s">
-        <v>261</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
+        <v>206</v>
+      </c>
+      <c r="J14" t="s">
         <v>207</v>
       </c>
-      <c r="H14" t="s">
-        <v>262</v>
-      </c>
-      <c r="I14" t="s">
-        <v>209</v>
-      </c>
-      <c r="J14" t="s">
-        <v>210</v>
-      </c>
       <c r="K14" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" t="s">
+        <v>261</v>
+      </c>
+      <c r="D15" t="s">
+        <v>243</v>
+      </c>
+      <c r="E15" t="s">
+        <v>262</v>
+      </c>
+      <c r="F15" t="s">
+        <v>203</v>
+      </c>
+      <c r="G15" t="s">
+        <v>204</v>
+      </c>
+      <c r="H15" t="s">
         <v>263</v>
       </c>
-      <c r="C15" t="s">
-        <v>264</v>
-      </c>
-      <c r="D15" t="s">
-        <v>246</v>
-      </c>
-      <c r="E15" t="s">
-        <v>265</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>206</v>
       </c>
-      <c r="G15" t="s">
+      <c r="J15" t="s">
         <v>207</v>
       </c>
-      <c r="H15" t="s">
-        <v>266</v>
-      </c>
-      <c r="I15" t="s">
-        <v>209</v>
-      </c>
-      <c r="J15" t="s">
-        <v>210</v>
-      </c>
       <c r="K15" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B16" t="s">
+        <v>264</v>
+      </c>
+      <c r="C16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D16" t="s">
+        <v>243</v>
+      </c>
+      <c r="E16" t="s">
+        <v>262</v>
+      </c>
+      <c r="F16" t="s">
+        <v>219</v>
+      </c>
+      <c r="G16" t="s">
+        <v>204</v>
+      </c>
+      <c r="H16" t="s">
+        <v>266</v>
+      </c>
+      <c r="I16" t="s">
         <v>267</v>
       </c>
-      <c r="C16" t="s">
-        <v>268</v>
-      </c>
-      <c r="D16" t="s">
-        <v>246</v>
-      </c>
-      <c r="E16" t="s">
-        <v>265</v>
-      </c>
-      <c r="F16" t="s">
-        <v>222</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="J16" t="s">
         <v>207</v>
       </c>
-      <c r="H16" t="s">
-        <v>269</v>
-      </c>
-      <c r="I16" t="s">
-        <v>270</v>
-      </c>
-      <c r="J16" t="s">
-        <v>210</v>
-      </c>
       <c r="K16" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B17" t="s">
+        <v>268</v>
+      </c>
+      <c r="C17" t="s">
+        <v>269</v>
+      </c>
+      <c r="D17" t="s">
+        <v>243</v>
+      </c>
+      <c r="E17" t="s">
+        <v>270</v>
+      </c>
+      <c r="F17" t="s">
+        <v>249</v>
+      </c>
+      <c r="G17" t="s">
+        <v>204</v>
+      </c>
+      <c r="H17" t="s">
         <v>271</v>
       </c>
-      <c r="C17" t="s">
-        <v>272</v>
-      </c>
-      <c r="D17" t="s">
-        <v>246</v>
-      </c>
-      <c r="E17" t="s">
-        <v>273</v>
-      </c>
-      <c r="F17" t="s">
-        <v>252</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
+        <v>206</v>
+      </c>
+      <c r="J17" t="s">
         <v>207</v>
       </c>
-      <c r="H17" t="s">
-        <v>274</v>
-      </c>
-      <c r="I17" t="s">
-        <v>209</v>
-      </c>
-      <c r="J17" t="s">
-        <v>210</v>
-      </c>
       <c r="K17" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B18" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C18" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E18" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F18" t="s">
+        <v>203</v>
+      </c>
+      <c r="G18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H18" t="s">
+        <v>274</v>
+      </c>
+      <c r="I18" t="s">
         <v>206</v>
       </c>
-      <c r="G18" t="s">
+      <c r="J18" t="s">
         <v>207</v>
       </c>
-      <c r="H18" t="s">
-        <v>277</v>
-      </c>
-      <c r="I18" t="s">
-        <v>209</v>
-      </c>
-      <c r="J18" t="s">
-        <v>210</v>
-      </c>
       <c r="K18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B19" t="s">
+        <v>275</v>
+      </c>
+      <c r="C19" t="s">
+        <v>276</v>
+      </c>
+      <c r="D19" t="s">
+        <v>201</v>
+      </c>
+      <c r="E19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F19" t="s">
+        <v>203</v>
+      </c>
+      <c r="G19" t="s">
+        <v>204</v>
+      </c>
+      <c r="H19" t="s">
         <v>278</v>
       </c>
-      <c r="C19" t="s">
-        <v>279</v>
-      </c>
-      <c r="D19" t="s">
-        <v>204</v>
-      </c>
-      <c r="E19" t="s">
-        <v>280</v>
-      </c>
-      <c r="F19" t="s">
-        <v>206</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
+        <v>267</v>
+      </c>
+      <c r="J19" t="s">
         <v>207</v>
       </c>
-      <c r="H19" t="s">
-        <v>281</v>
-      </c>
-      <c r="I19" t="s">
-        <v>270</v>
-      </c>
-      <c r="J19" t="s">
-        <v>210</v>
-      </c>
       <c r="K19" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s">
+        <v>279</v>
+      </c>
+      <c r="C20" t="s">
+        <v>280</v>
+      </c>
+      <c r="D20" t="s">
+        <v>201</v>
+      </c>
+      <c r="E20" t="s">
+        <v>281</v>
+      </c>
+      <c r="F20" t="s">
         <v>282</v>
       </c>
-      <c r="C20" t="s">
+      <c r="G20" t="s">
+        <v>204</v>
+      </c>
+      <c r="H20" t="s">
         <v>283</v>
       </c>
-      <c r="D20" t="s">
-        <v>204</v>
-      </c>
-      <c r="E20" t="s">
-        <v>284</v>
-      </c>
-      <c r="F20" t="s">
-        <v>285</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="I20" t="s">
+        <v>267</v>
+      </c>
+      <c r="J20" t="s">
         <v>207</v>
       </c>
-      <c r="H20" t="s">
-        <v>286</v>
-      </c>
-      <c r="I20" t="s">
-        <v>270</v>
-      </c>
-      <c r="J20" t="s">
-        <v>210</v>
-      </c>
       <c r="K20" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B21" t="s">
+        <v>284</v>
+      </c>
+      <c r="C21" t="s">
+        <v>285</v>
+      </c>
+      <c r="D21" t="s">
+        <v>286</v>
+      </c>
+      <c r="E21" t="s">
         <v>287</v>
       </c>
-      <c r="C21" t="s">
+      <c r="F21" t="s">
+        <v>219</v>
+      </c>
+      <c r="G21" t="s">
+        <v>204</v>
+      </c>
+      <c r="H21" t="s">
         <v>288</v>
       </c>
-      <c r="D21" t="s">
-        <v>289</v>
-      </c>
-      <c r="E21" t="s">
-        <v>290</v>
-      </c>
-      <c r="F21" t="s">
-        <v>222</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
+        <v>267</v>
+      </c>
+      <c r="J21" t="s">
         <v>207</v>
       </c>
-      <c r="H21" t="s">
-        <v>291</v>
-      </c>
-      <c r="I21" t="s">
-        <v>270</v>
-      </c>
-      <c r="J21" t="s">
-        <v>210</v>
-      </c>
       <c r="K21" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -4207,10 +4183,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A2CF0A-0BF8-448E-99C2-57F5D470810B}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4230,55 +4206,55 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4286,171 +4262,157 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>36</v>
+        <v>139</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>171</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>48</v>
+        <v>356</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>60</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>174</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>363</v>
-      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>321</v>
+        <v>47</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>302</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>42</v>
+        <v>4</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>171</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>44</v>
+        <v>133</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>54</v>
+        <v>302</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>174</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{517CE8C8-60D2-43EA-919E-915C552D3875}"/>
+    <hyperlink ref="B15" r:id="rId1" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{517CE8C8-60D2-43EA-919E-915C552D3875}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated new List of Prod Tmp conservation files
</commit_message>
<xml_diff>
--- a/analysis/Current-Historical-List-Ids.xlsx
+++ b/analysis/Current-Historical-List-Ids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oco115\PycharmProjects\authoritative-lists\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9F41FD-6434-4515-B5D7-C143325066C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602E1A30-4B23-4EA5-ABDF-97DD257589E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="2850" windowWidth="29925" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15690" yWindow="2535" windowWidth="34125" windowHeight="18465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="File Summary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="377">
   <si>
     <t>Sensitive</t>
   </si>
@@ -1108,13 +1108,64 @@
   </si>
   <si>
     <t>dr18782</t>
+  </si>
+  <si>
+    <t>New list but not tested</t>
+  </si>
+  <si>
+    <t>dr18973</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18973</t>
+  </si>
+  <si>
+    <t>BONN</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18974</t>
+  </si>
+  <si>
+    <t>dr18974</t>
+  </si>
+  <si>
+    <t>CAMBA</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18975</t>
+  </si>
+  <si>
+    <t>dr18975</t>
+  </si>
+  <si>
+    <t>JAMBA</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18976</t>
+  </si>
+  <si>
+    <t>dr18976</t>
+  </si>
+  <si>
+    <t>ROKAMBA</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18977</t>
+  </si>
+  <si>
+    <t>dr18977</t>
+  </si>
+  <si>
+    <t>https://lists.ala.org.au/speciesListItem/list/dr18980</t>
+  </si>
+  <si>
+    <t>dr18980</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1194,6 +1245,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1246,7 +1312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1269,6 +1335,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1550,16 +1618,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="50.42578125" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="54.140625" customWidth="1"/>
@@ -1749,7 +1816,7 @@
         <v>149</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>174</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2082,17 +2149,20 @@
       </c>
     </row>
     <row r="36" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="F36" s="7" t="s">
-        <v>174</v>
+      <c r="E36" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2138,220 +2208,281 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D40" s="4"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B42" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D42" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F42" s="10" t="s">
         <v>299</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="F42" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F43" t="s">
-        <v>300</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F44" t="s">
-        <v>59</v>
+        <v>300</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F45" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>41</v>
+        <v>313</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F46" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>43</v>
+        <v>314</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>171</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="50" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="D50" s="19" t="s">
+      <c r="D51" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="E50" s="18"/>
-      <c r="G50" s="8" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="E51" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="C52" s="18"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="7" t="s">
+    <row r="60" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D60" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E60" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F60" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="7" t="s">
+    <row r="62" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D62" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E62" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="F56" s="7" t="s">
+      <c r="F62" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G56" s="7" t="s">
+      <c r="G62" s="7" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2362,44 +2493,44 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{952BDF74-1025-44CA-B437-CA7A782DEF2C}"/>
     <hyperlink ref="D20" r:id="rId3" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BA5A33AF-C0B9-4DFE-9F12-7BFDF7D8A911}"/>
     <hyperlink ref="E23" r:id="rId4" xr:uid="{ECFB10CF-9B59-4B58-9F8C-86B26ED2D1A6}"/>
-    <hyperlink ref="C46" r:id="rId5" xr:uid="{D698F75E-C3A9-2E43-9EF9-D03CAFBC8EA9}"/>
+    <hyperlink ref="C47" r:id="rId5" xr:uid="{D698F75E-C3A9-2E43-9EF9-D03CAFBC8EA9}"/>
     <hyperlink ref="C29" r:id="rId6" display="https://lists-test.ala.org.au/speciesListItem/list/dr2627" xr:uid="{4780244B-70BF-9C48-970A-9B52EE257B77}"/>
-    <hyperlink ref="D46" r:id="rId7" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BCC2EF75-48CD-4548-9585-233F9187C820}"/>
+    <hyperlink ref="D47" r:id="rId7" display="https://lists-test.ala.org.au/speciesListItem/list/dr654" xr:uid="{BCC2EF75-48CD-4548-9585-233F9187C820}"/>
     <hyperlink ref="A28" r:id="rId8" xr:uid="{4A0B836D-E3B0-794C-A4F5-21AA69E861E2}"/>
     <hyperlink ref="A2" r:id="rId9" xr:uid="{6FC89B14-CCA6-C244-9CDE-F11F9F1FF7E7}"/>
     <hyperlink ref="A15" r:id="rId10" xr:uid="{6366CB73-381F-0249-A1E4-038947A0C509}"/>
-    <hyperlink ref="A41" r:id="rId11" xr:uid="{B8D63856-57FE-8C42-8EAD-AECB4BC1FF98}"/>
-    <hyperlink ref="C41" r:id="rId12" xr:uid="{96429AFB-B264-344B-B15E-8F464D602044}"/>
-    <hyperlink ref="C42" r:id="rId13" xr:uid="{31C2BC7F-43DC-0447-95EB-1702F49CA889}"/>
-    <hyperlink ref="C43" r:id="rId14" xr:uid="{5EF5C7C0-C9E6-624F-BF44-A5738449F8BA}"/>
-    <hyperlink ref="C44" r:id="rId15" xr:uid="{9AA0D4E8-104C-FA40-B731-F1AFD127B25C}"/>
-    <hyperlink ref="C45" r:id="rId16" xr:uid="{0AA1FC7B-6EFA-B54C-A968-3E6832124A77}"/>
-    <hyperlink ref="C47" r:id="rId17" xr:uid="{88BF66EA-B4A9-5B40-A7A3-599D95618642}"/>
-    <hyperlink ref="C48" r:id="rId18" xr:uid="{7A14450F-9C85-3C46-891C-D60F0551E9B5}"/>
+    <hyperlink ref="A42" r:id="rId11" xr:uid="{B8D63856-57FE-8C42-8EAD-AECB4BC1FF98}"/>
+    <hyperlink ref="C42" r:id="rId12" xr:uid="{96429AFB-B264-344B-B15E-8F464D602044}"/>
+    <hyperlink ref="C43" r:id="rId13" xr:uid="{31C2BC7F-43DC-0447-95EB-1702F49CA889}"/>
+    <hyperlink ref="C44" r:id="rId14" xr:uid="{5EF5C7C0-C9E6-624F-BF44-A5738449F8BA}"/>
+    <hyperlink ref="C45" r:id="rId15" xr:uid="{9AA0D4E8-104C-FA40-B731-F1AFD127B25C}"/>
+    <hyperlink ref="C46" r:id="rId16" xr:uid="{0AA1FC7B-6EFA-B54C-A968-3E6832124A77}"/>
+    <hyperlink ref="C48" r:id="rId17" xr:uid="{88BF66EA-B4A9-5B40-A7A3-599D95618642}"/>
+    <hyperlink ref="C49" r:id="rId18" xr:uid="{7A14450F-9C85-3C46-891C-D60F0551E9B5}"/>
     <hyperlink ref="C24" r:id="rId19" xr:uid="{5A2DA5AE-E509-094D-981A-96E4E13B0899}"/>
     <hyperlink ref="C31" r:id="rId20" display="https://lists-test.ala.org.au/speciesListItem/list/dr490" xr:uid="{E684EDD1-59E8-432F-83AA-222E20CB276C}"/>
     <hyperlink ref="E30" r:id="rId21" xr:uid="{8B4FF377-6E00-4C40-A026-AC534597AF83}"/>
     <hyperlink ref="E31" r:id="rId22" xr:uid="{5DCC8A3F-A15F-4D27-9655-D103A175BED4}"/>
     <hyperlink ref="E39" r:id="rId23" xr:uid="{7A373A1D-1D80-4574-9F0E-6361ADE6EA1B}"/>
-    <hyperlink ref="E41" r:id="rId24" xr:uid="{D774CFC5-AE6A-4609-9ADC-A7D7C699A6EB}"/>
-    <hyperlink ref="E42" r:id="rId25" xr:uid="{007E7E11-1D71-43C4-A264-4660FCB67FAC}"/>
-    <hyperlink ref="E43" r:id="rId26" xr:uid="{42F37AA5-D002-41C0-B5CE-B2C89A43B972}"/>
-    <hyperlink ref="E44" r:id="rId27" xr:uid="{FE56801B-7C8F-41C7-A5B5-35433F8B885F}"/>
-    <hyperlink ref="E45" r:id="rId28" xr:uid="{13D8FFBA-7AD0-4D3F-ADA5-3DA7818D2543}"/>
-    <hyperlink ref="E46" r:id="rId29" xr:uid="{1999C80C-0543-421A-9E09-CE6EC8403DBC}"/>
-    <hyperlink ref="E47" r:id="rId30" xr:uid="{CDEA47CE-620A-46F0-80F6-04AB3B2B19E0}"/>
-    <hyperlink ref="E48" r:id="rId31" xr:uid="{F8B85F77-E546-4150-86A7-B0F301B0C6F3}"/>
+    <hyperlink ref="E42" r:id="rId24" xr:uid="{D774CFC5-AE6A-4609-9ADC-A7D7C699A6EB}"/>
+    <hyperlink ref="E43" r:id="rId25" xr:uid="{007E7E11-1D71-43C4-A264-4660FCB67FAC}"/>
+    <hyperlink ref="E44" r:id="rId26" xr:uid="{42F37AA5-D002-41C0-B5CE-B2C89A43B972}"/>
+    <hyperlink ref="E45" r:id="rId27" xr:uid="{FE56801B-7C8F-41C7-A5B5-35433F8B885F}"/>
+    <hyperlink ref="E46" r:id="rId28" xr:uid="{13D8FFBA-7AD0-4D3F-ADA5-3DA7818D2543}"/>
+    <hyperlink ref="E47" r:id="rId29" xr:uid="{1999C80C-0543-421A-9E09-CE6EC8403DBC}"/>
+    <hyperlink ref="E48" r:id="rId30" xr:uid="{CDEA47CE-620A-46F0-80F6-04AB3B2B19E0}"/>
+    <hyperlink ref="E49" r:id="rId31" xr:uid="{F8B85F77-E546-4150-86A7-B0F301B0C6F3}"/>
     <hyperlink ref="C11" r:id="rId32" xr:uid="{FE96DD95-E99E-4362-A5D5-4B69BAAB8B58}"/>
     <hyperlink ref="C12" r:id="rId33" xr:uid="{B3C11E20-1B34-458E-8A79-AABFC15FBBF8}"/>
     <hyperlink ref="C13" r:id="rId34" xr:uid="{FBABA9A6-5AD3-4585-AACA-D7F375DF505C}"/>
     <hyperlink ref="C35" r:id="rId35" display="https://lists-test.ala.org.au/speciesListItem/list/dr492" xr:uid="{5ADFD62E-071D-4D50-A9F1-7DD045E02C7D}"/>
     <hyperlink ref="C36" r:id="rId36" display="https://lists-test.ala.org.au/speciesListItem/list/dr884" xr:uid="{8135FF93-4DC0-49ED-B2EC-9F87EC85B79E}"/>
     <hyperlink ref="C37" r:id="rId37" display="https://lists-test.ala.org.au/speciesListItem/list/dr491" xr:uid="{0FA25B88-5583-4A34-91A9-8293F79F5C17}"/>
-    <hyperlink ref="C32:C54" r:id="rId38" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{5E1A38EB-C2FC-4CB9-95BD-919CFF22EC41}"/>
+    <hyperlink ref="C32:C60" r:id="rId38" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{5E1A38EB-C2FC-4CB9-95BD-919CFF22EC41}"/>
     <hyperlink ref="C32" r:id="rId39" xr:uid="{2A8CE89C-4876-4A29-B6EB-5A9A6FED5677}"/>
     <hyperlink ref="C33" r:id="rId40" xr:uid="{F58F9C57-D04A-4DFB-A449-5C8B903F4512}"/>
-    <hyperlink ref="C54" r:id="rId41" xr:uid="{A21E7F06-2AF5-4850-985F-BB2E6FD743BB}"/>
-    <hyperlink ref="C56" r:id="rId42" xr:uid="{6471530C-DA5E-43A6-B7BA-36E8172AC848}"/>
+    <hyperlink ref="C60" r:id="rId41" xr:uid="{A21E7F06-2AF5-4850-985F-BB2E6FD743BB}"/>
+    <hyperlink ref="C62" r:id="rId42" xr:uid="{6471530C-DA5E-43A6-B7BA-36E8172AC848}"/>
     <hyperlink ref="C34" r:id="rId43" xr:uid="{0A7CD882-4D7D-4020-A769-C978BA913387}"/>
     <hyperlink ref="C6:C7" r:id="rId44" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{BF20DF31-07E8-4589-A04E-683DB3D80B17}"/>
     <hyperlink ref="C6" r:id="rId45" xr:uid="{DFF57021-8E37-4EB9-8920-609DB7F6AE09}"/>
@@ -2410,9 +2541,19 @@
     <hyperlink ref="E8" r:id="rId50" xr:uid="{9E262E71-4F7D-4CCE-A7C4-371E3CC124B6}"/>
     <hyperlink ref="E34" r:id="rId51" xr:uid="{C2D49F08-150A-46F1-B8D5-876F1ACE8778}"/>
     <hyperlink ref="E10" r:id="rId52" xr:uid="{8D5650F4-48BD-465C-881F-2A05C01FAB4D}"/>
+    <hyperlink ref="E52" r:id="rId53" xr:uid="{947C389C-6829-42AD-ADB2-28C87EE85E93}"/>
+    <hyperlink ref="C53" r:id="rId54" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{0921F00A-6DAB-4050-BE45-A5EFBA57B48A}"/>
+    <hyperlink ref="E53" r:id="rId55" xr:uid="{7CF2E72D-B4E2-4819-BA99-34247612D2FE}"/>
+    <hyperlink ref="C54" r:id="rId56" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{776573F7-01A2-47A5-A58B-256DE287A2F8}"/>
+    <hyperlink ref="E54" r:id="rId57" xr:uid="{5C9DDA4C-50B0-4BB9-A5CE-880F36D9BC34}"/>
+    <hyperlink ref="C55" r:id="rId58" display="https://lists.ala.org.au/speciesListItem/list/dr649" xr:uid="{95D94539-2454-49BF-A818-709583A8F14A}"/>
+    <hyperlink ref="E55" r:id="rId59" xr:uid="{3D92EDC9-C004-48E9-A678-A9AFDA6D0A98}"/>
+    <hyperlink ref="E36" r:id="rId60" xr:uid="{981CE5C4-5CBD-4851-845D-A1C9C24B5CD8}"/>
+    <hyperlink ref="E50" r:id="rId61" xr:uid="{DE8417C0-08C6-41E9-8C2B-1BA7C62CFFB6}"/>
+    <hyperlink ref="E51" r:id="rId62" xr:uid="{68C7F76C-FEC7-4531-B6D6-B771B84FA6F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId53"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId63"/>
 </worksheet>
 </file>
 

</xml_diff>